<commit_message>
update nlcdLandCover README & status file
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="267">
   <si>
     <t>forest</t>
   </si>
@@ -193,16 +193,7 @@
     <t>"SLOPE"</t>
   </si>
   <si>
-    <t>UndevelopedForest</t>
-  </si>
-  <si>
     <t>Impervious</t>
-  </si>
-  <si>
-    <t>Wetland</t>
-  </si>
-  <si>
-    <t>Water</t>
   </si>
   <si>
     <t>CONUSOpenWater</t>
@@ -472,18 +463,6 @@
     <t>Percent Developed, Open</t>
   </si>
   <si>
-    <t>DevelopedHigh</t>
-  </si>
-  <si>
-    <t>DevelopedMedium</t>
-  </si>
-  <si>
-    <t>DevelopedLow</t>
-  </si>
-  <si>
-    <t>DevelopedOpen</t>
-  </si>
-  <si>
     <t>Percent Deciduous Forest</t>
   </si>
   <si>
@@ -491,15 +470,6 @@
   </si>
   <si>
     <t>Percent Mixed Forest</t>
-  </si>
-  <si>
-    <t>ForestDeciduous</t>
-  </si>
-  <si>
-    <t>ForestEvergreen</t>
-  </si>
-  <si>
-    <t>ForestMixed</t>
   </si>
   <si>
     <t>Deciduous Forest (41)</t>
@@ -812,10 +782,55 @@
     <t>Percent Developed</t>
   </si>
   <si>
-    <t>Developed, Open Space(21), Developed, Low Intensity (22), Developed, Medium Intensity (23), Developed, High Intensity (24), Unconsolidated Shore/Quarries/Gravel Pits/Strip Mines(32)</t>
-  </si>
-  <si>
     <t>developed</t>
+  </si>
+  <si>
+    <t>Automated Raster Prep</t>
+  </si>
+  <si>
+    <t>forest_decid</t>
+  </si>
+  <si>
+    <t>forest_evgrn</t>
+  </si>
+  <si>
+    <t>forest_mixed</t>
+  </si>
+  <si>
+    <t>undev_forest</t>
+  </si>
+  <si>
+    <t>agriculture</t>
+  </si>
+  <si>
+    <t>devel_opn</t>
+  </si>
+  <si>
+    <t>devel_low</t>
+  </si>
+  <si>
+    <t>devel_med</t>
+  </si>
+  <si>
+    <t>devel_hi</t>
+  </si>
+  <si>
+    <t>wetland</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Percent Agriculture</t>
+  </si>
+  <si>
+    <t>Percent Herbaceous</t>
+  </si>
+  <si>
+    <t>herbaceous</t>
+  </si>
+  <si>
+    <t>"Land_Cover" (Land Cover Class) Developed, Open Space(21), Developed, Low Intensity (22), Developed, Medium Intensity (23), Developed, High Intensity (24), Unconsolidated Shore/Quarries/Gravel Pits/Strip Mines(32), Urban/Recreational Grasses (85)</t>
   </si>
 </sst>
 </file>
@@ -894,7 +909,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -963,11 +978,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,9 +1088,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1094,11 +1143,72 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1859,30 +1969,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:U68" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
-  <autoFilter ref="A1:U68"/>
-  <tableColumns count="21">
-    <tableColumn id="1" name="Data Layer" dataDxfId="21"/>
-    <tableColumn id="9" name="Description" dataDxfId="20"/>
-    <tableColumn id="18" name="Name" dataDxfId="19"/>
-    <tableColumn id="5" name="Data Source" dataDxfId="18"/>
-    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="17"/>
-    <tableColumn id="3" name="Final Units" dataDxfId="16"/>
-    <tableColumn id="6" name="Layer Classification" dataDxfId="15"/>
-    <tableColumn id="19" name="Local" dataDxfId="14"/>
-    <tableColumn id="20" name="Upstream" dataDxfId="13"/>
-    <tableColumn id="10" name="CT" dataDxfId="12"/>
-    <tableColumn id="11" name="DC" dataDxfId="11"/>
-    <tableColumn id="8" name="DE" dataDxfId="10"/>
-    <tableColumn id="12" name="MA" dataDxfId="9"/>
-    <tableColumn id="7" name="MD" dataDxfId="8"/>
-    <tableColumn id="13" name="ME" dataDxfId="7"/>
-    <tableColumn id="14" name="NJ" dataDxfId="6"/>
-    <tableColumn id="15" name="NY" dataDxfId="5"/>
-    <tableColumn id="24" name="PA" dataDxfId="4"/>
-    <tableColumn id="23" name="VA" dataDxfId="3"/>
-    <tableColumn id="17" name="VT" dataDxfId="2"/>
-    <tableColumn id="16" name="WV" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:V70" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
+  <autoFilter ref="A1:V70"/>
+  <tableColumns count="22">
+    <tableColumn id="1" name="Data Layer" dataDxfId="22"/>
+    <tableColumn id="9" name="Description" dataDxfId="21"/>
+    <tableColumn id="18" name="Name" dataDxfId="20"/>
+    <tableColumn id="5" name="Data Source" dataDxfId="19"/>
+    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="18"/>
+    <tableColumn id="3" name="Final Units" dataDxfId="17"/>
+    <tableColumn id="6" name="Layer Classification" dataDxfId="16"/>
+    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="0"/>
+    <tableColumn id="19" name="Local" dataDxfId="15"/>
+    <tableColumn id="20" name="Upstream" dataDxfId="14"/>
+    <tableColumn id="10" name="CT" dataDxfId="13"/>
+    <tableColumn id="11" name="DC" dataDxfId="12"/>
+    <tableColumn id="8" name="DE" dataDxfId="11"/>
+    <tableColumn id="12" name="MA" dataDxfId="10"/>
+    <tableColumn id="7" name="MD" dataDxfId="9"/>
+    <tableColumn id="13" name="ME" dataDxfId="8"/>
+    <tableColumn id="14" name="NJ" dataDxfId="7"/>
+    <tableColumn id="15" name="NY" dataDxfId="6"/>
+    <tableColumn id="24" name="PA" dataDxfId="5"/>
+    <tableColumn id="23" name="VA" dataDxfId="4"/>
+    <tableColumn id="17" name="VT" dataDxfId="3"/>
+    <tableColumn id="16" name="WV" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1893,7 +2004,7 @@
   <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Data Source"/>
-    <tableColumn id="2" name="Data Source Description" dataDxfId="0"/>
+    <tableColumn id="2" name="Data Source Description" dataDxfId="1"/>
     <tableColumn id="4" name="Raw Data Layer"/>
     <tableColumn id="3" name="Data Source File Path"/>
   </tableColumns>
@@ -2191,13 +2302,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V68"/>
+  <dimension ref="A1:W70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -2209,171 +2320,178 @@
     <col min="5" max="5" width="86" style="20" customWidth="1"/>
     <col min="6" max="6" width="23" style="21" customWidth="1"/>
     <col min="7" max="7" width="70.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="18" style="10" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="24" customWidth="1"/>
-    <col min="11" max="11" width="10" style="24" customWidth="1"/>
-    <col min="12" max="12" width="11" style="24" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="24" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="24" customWidth="1"/>
-    <col min="17" max="18" width="8.140625" style="24" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" style="24" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" style="24" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" style="24" customWidth="1"/>
-    <col min="22" max="22" width="24" style="24" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="18" style="10" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="24" customWidth="1"/>
+    <col min="12" max="12" width="10" style="24" customWidth="1"/>
+    <col min="13" max="13" width="11" style="24" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="24" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" style="24" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" style="24" customWidth="1"/>
+    <col min="18" max="19" width="8.140625" style="24" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="24" customWidth="1"/>
+    <col min="21" max="21" width="7.85546875" style="24" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" style="24" customWidth="1"/>
+    <col min="23" max="23" width="24" style="24" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="11" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="O1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="Q1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="S1" s="5" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="T1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="V1" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V2"/>
-    </row>
-    <row r="3" spans="1:22" ht="93" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="1:23" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>29</v>
@@ -2382,720 +2500,753 @@
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V3"/>
-    </row>
-    <row r="4" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V4"/>
-    </row>
-    <row r="5" spans="1:22" ht="93" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="1:23" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V5"/>
-    </row>
-    <row r="6" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V6"/>
-    </row>
-    <row r="7" spans="1:22" ht="119.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:23" ht="119.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V7"/>
-    </row>
-    <row r="8" spans="1:22" ht="117.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="1:23" ht="117.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V8"/>
-    </row>
-    <row r="9" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="K9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W10"/>
+    </row>
+    <row r="11" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="H11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V9"/>
-    </row>
-    <row r="10" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="33" t="s">
+      <c r="E12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="H12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W12"/>
+    </row>
+    <row r="13" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V10"/>
-    </row>
-    <row r="11" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="33" t="s">
+      <c r="E13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V11"/>
-    </row>
-    <row r="12" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V12"/>
-    </row>
-    <row r="13" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>192</v>
+      <c r="H13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="V13"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="W13"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="12"/>
-      <c r="B14" s="35"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="36"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="18"/>
       <c r="F14" s="13"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -3107,55 +3258,59 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14"/>
-    </row>
-    <row r="15" spans="1:22" s="45" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-    </row>
-    <row r="16" spans="1:22" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="V14" s="2"/>
+      <c r="W14"/>
+    </row>
+    <row r="15" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+    </row>
+    <row r="16" spans="1:23" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D16" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="D16" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>167</v>
+      <c r="E16" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="H16" s="7"/>
+        <v>266</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -3166,21 +3321,22 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-      <c r="V16"/>
-    </row>
-    <row r="17" spans="1:22" ht="93" x14ac:dyDescent="0.35">
+      <c r="V16" s="3"/>
+      <c r="W16"/>
+    </row>
+    <row r="17" spans="1:23" ht="93" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>167</v>
+      <c r="E17" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>29</v>
@@ -3188,10 +3344,12 @@
       <c r="G17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="I17" s="8"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -3202,32 +3360,35 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V17" s="3"/>
+      <c r="W17"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>167</v>
+      <c r="E18" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
+      <c r="G18" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -3237,33 +3398,36 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="28"/>
-      <c r="V18"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U18" s="3"/>
+      <c r="V18" s="27"/>
+      <c r="W18"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="D19" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>167</v>
+      <c r="E19" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="3"/>
+      <c r="G19" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -3273,33 +3437,36 @@
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-      <c r="U19" s="28"/>
-      <c r="V19"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U19" s="3"/>
+      <c r="V19" s="27"/>
+      <c r="W19"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>167</v>
+      <c r="E20" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="3"/>
+      <c r="G20" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -3309,33 +3476,36 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-      <c r="U20" s="28"/>
-      <c r="V20"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U20" s="3"/>
+      <c r="V20" s="27"/>
+      <c r="W20"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D21" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="53" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>167</v>
+      <c r="E21" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
+        <v>149</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -3345,33 +3515,36 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="28"/>
-      <c r="V21"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U21" s="3"/>
+      <c r="V21" s="27"/>
+      <c r="W21"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="53" t="s">
+        <v>252</v>
+      </c>
+      <c r="D22" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>167</v>
+      <c r="E22" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
+      <c r="G22" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="2"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -3381,33 +3554,36 @@
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="28"/>
-      <c r="V22"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U22" s="3"/>
+      <c r="V22" s="27"/>
+      <c r="W22"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="D23" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>167</v>
+      <c r="E23" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="3"/>
+      <c r="G23" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="2"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -3417,33 +3593,36 @@
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="28"/>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="U23" s="3"/>
+      <c r="V23" s="27"/>
+      <c r="W23"/>
+    </row>
+    <row r="24" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="51"/>
+      <c r="C24" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>167</v>
+      <c r="E24" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
+      <c r="G24" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -3453,33 +3632,36 @@
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="28"/>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="1:22" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U24" s="3"/>
+      <c r="V24" s="27"/>
+      <c r="W24"/>
+    </row>
+    <row r="25" spans="1:23" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="50"/>
+      <c r="C25" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>29</v>
+      <c r="E25" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H25" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="I25" s="8"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="3"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -3490,32 +3672,34 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-      <c r="V25"/>
-    </row>
-    <row r="26" spans="1:22" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V25" s="3"/>
+    </row>
+    <row r="26" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>167</v>
+      <c r="E26" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="I26" s="8"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -3526,244 +3710,250 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="V26" s="3"/>
+    </row>
+    <row r="27" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B27" s="46"/>
+      <c r="C27" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="D27" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>167</v>
+      <c r="E27" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="47"/>
+      <c r="H27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="49"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>167</v>
+        <v>263</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28"/>
-    </row>
-    <row r="29" spans="1:22" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28"/>
+      <c r="H28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="49"/>
+      <c r="W28"/>
+    </row>
+    <row r="29" spans="1:23" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="B29" s="50"/>
       <c r="C29" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="2"/>
+      <c r="G29" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
-      <c r="V29"/>
-    </row>
-    <row r="30" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29"/>
+    </row>
+    <row r="30" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="23" t="s">
-        <v>93</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H30" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="H30" s="2"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="2"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
-      <c r="V30"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V30" s="3"/>
+      <c r="W30"/>
+    </row>
+    <row r="31" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="8" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H31" s="2"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
-      <c r="V31"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W31"/>
+    </row>
+    <row r="32" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="8" t="s">
-        <v>126</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H32" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H32" s="2"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
-      <c r="V32"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H33" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H33" s="2"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -3774,32 +3964,33 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
-      <c r="V33"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V33" s="3"/>
+      <c r="W33"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="8" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H34" s="2"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="3"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="2"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -3810,32 +4001,32 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
-      <c r="V34"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W34"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="8" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H35" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H35" s="2"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="3"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="2"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -3845,15 +4036,17 @@
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
-      <c r="V35"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="23" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>7</v>
@@ -3865,12 +4058,12 @@
         <v>34</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H36" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H36" s="2"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="3"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="2"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -3881,15 +4074,16 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
-      <c r="V36"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V36" s="3"/>
+      <c r="W36"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>7</v>
@@ -3901,12 +4095,12 @@
         <v>34</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H37" s="2"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="3"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -3917,15 +4111,15 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
-      <c r="V37"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W37"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="23" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>7</v>
@@ -3937,12 +4131,12 @@
         <v>34</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H38" s="2"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="3"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="2"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -3952,15 +4146,17 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
-      <c r="V38"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="23" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>7</v>
@@ -3972,12 +4168,12 @@
         <v>34</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H39" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H39" s="2"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="3"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -3988,15 +4184,16 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
-      <c r="V39"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V39" s="3"/>
+      <c r="W39"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="23" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>7</v>
@@ -4008,12 +4205,12 @@
         <v>34</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H40" s="2"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="3"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="2"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -4024,15 +4221,15 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
-      <c r="V40"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W40"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>7</v>
@@ -4044,12 +4241,12 @@
         <v>34</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H41" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="3"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="2"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -4059,15 +4256,17 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
-      <c r="V41"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="23" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>7</v>
@@ -4079,12 +4278,12 @@
         <v>34</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H42" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H42" s="2"/>
       <c r="I42" s="7"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="3"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="2"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -4095,15 +4294,16 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
-      <c r="V42"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V42" s="3"/>
+      <c r="W42"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B43" s="14"/>
       <c r="C43" s="23" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>7</v>
@@ -4115,12 +4315,12 @@
         <v>34</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H43" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H43" s="2"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="3"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="2"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -4131,15 +4331,15 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
-      <c r="V43"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W43"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>7</v>
@@ -4151,12 +4351,12 @@
         <v>34</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H44" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H44" s="2"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="3"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="2"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -4166,15 +4366,17 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
-      <c r="V44"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>7</v>
@@ -4186,12 +4388,12 @@
         <v>34</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H45" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H45" s="2"/>
       <c r="I45" s="7"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="3"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="2"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -4202,15 +4404,16 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
-      <c r="V45"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V45" s="3"/>
+      <c r="W45"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>7</v>
@@ -4222,12 +4425,12 @@
         <v>34</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H46" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H46" s="2"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="3"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="2"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -4238,15 +4441,15 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
-      <c r="V46"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W46"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -4258,12 +4461,12 @@
         <v>34</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H47" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H47" s="2"/>
       <c r="I47" s="7"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="3"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="2"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -4273,15 +4476,17 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
-      <c r="V47"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="23" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>7</v>
@@ -4293,12 +4498,12 @@
         <v>34</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H48" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H48" s="2"/>
       <c r="I48" s="7"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="3"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="2"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -4309,15 +4514,16 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
-      <c r="V48"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V48" s="3"/>
+      <c r="W48"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>7</v>
@@ -4329,12 +4535,12 @@
         <v>34</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H49" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H49" s="2"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="3"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="2"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -4345,68 +4551,69 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
-      <c r="V49"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W49"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="8" t="s">
-        <v>62</v>
+        <v>108</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>167</v>
+        <v>34</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H50" s="2"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="2"/>
+      <c r="J50" s="7"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
-      <c r="V50"/>
-    </row>
-    <row r="51" spans="1:22" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="V50" s="3"/>
+      <c r="W50"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="8" t="s">
-        <v>63</v>
+        <v>109</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H51" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H51" s="2"/>
       <c r="I51" s="7"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -4416,31 +4623,33 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
-      <c r="V51"/>
-    </row>
-    <row r="52" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H52" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="H52" s="2"/>
       <c r="I52" s="7"/>
-      <c r="J52" s="2"/>
+      <c r="J52" s="7"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
@@ -4448,71 +4657,72 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
-      <c r="R52" s="3"/>
+      <c r="R52" s="2"/>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
-      <c r="V52"/>
-    </row>
-    <row r="53" spans="1:22" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="V52" s="3"/>
+      <c r="W52"/>
+    </row>
+    <row r="53" spans="1:23" ht="162.75" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>167</v>
+        <v>35</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H53" s="7"/>
+        <v>126</v>
+      </c>
+      <c r="H53" s="2"/>
       <c r="I53" s="7"/>
-      <c r="J53" s="2"/>
+      <c r="J53" s="7"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
-      <c r="V53"/>
-    </row>
-    <row r="54" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="W53"/>
+    </row>
+    <row r="54" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H54" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="H54" s="2"/>
       <c r="I54" s="7"/>
-      <c r="J54" s="2"/>
+      <c r="J54" s="7"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
@@ -4520,34 +4730,36 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="3"/>
+      <c r="R54" s="2"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
-      <c r="V54"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54"/>
+    </row>
+    <row r="55" spans="1:23" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H55" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="H55" s="2"/>
       <c r="I55" s="7"/>
-      <c r="J55" s="2"/>
+      <c r="J55" s="7"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -4555,35 +4767,36 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="3"/>
+      <c r="R55" s="2"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
-      <c r="V55"/>
-    </row>
-    <row r="56" spans="1:22" ht="93" x14ac:dyDescent="0.35">
+      <c r="V55" s="3"/>
+      <c r="W55"/>
+    </row>
+    <row r="56" spans="1:23" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F56" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H56" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="H56" s="2"/>
       <c r="I56" s="7"/>
-      <c r="J56" s="2"/>
+      <c r="J56" s="7"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -4591,177 +4804,182 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="3"/>
+      <c r="R56" s="2"/>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
-      <c r="V56"/>
-    </row>
-    <row r="57" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="W56"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H57" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="H57" s="2"/>
       <c r="I57" s="7"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
-      <c r="V57"/>
-    </row>
-    <row r="58" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57"/>
+    </row>
+    <row r="58" spans="1:23" ht="93" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H58" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="H58" s="2"/>
       <c r="I58" s="7"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
-      <c r="V58"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V58" s="3"/>
+      <c r="W58"/>
+    </row>
+    <row r="59" spans="1:23" ht="93" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>142</v>
+        <v>66</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="E59" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H59" s="2"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="W59"/>
+    </row>
+    <row r="60" spans="1:23" ht="93" x14ac:dyDescent="0.35">
+      <c r="A60" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H60" s="2"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A61" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F61" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G59" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="2"/>
-      <c r="U59" s="3"/>
-      <c r="V59"/>
-    </row>
-    <row r="60" spans="1:22" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="23"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="2"/>
-      <c r="S60" s="2"/>
-      <c r="T60" s="2"/>
-      <c r="V60"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A61" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="15"/>
-      <c r="C61" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="2"/>
+      <c r="G61" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -4772,67 +4990,69 @@
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-      <c r="U61" s="3"/>
-      <c r="V61"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A62" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="12"/>
-      <c r="C62" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="F62" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61" s="3"/>
+      <c r="W61"/>
+    </row>
+    <row r="62" spans="1:23" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A62" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="22"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
-      <c r="V62"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="U62" s="2"/>
+      <c r="W62"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A63" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="2"/>
+      <c r="E63" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -4843,65 +5063,69 @@
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
-      <c r="U63" s="3"/>
-      <c r="V63"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U63" s="2"/>
+      <c r="V63" s="3"/>
+      <c r="W63"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="14"/>
-      <c r="C64" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D64" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E64" s="13" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="H64" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="H64" s="2"/>
       <c r="I64" s="7"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
-      <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="J64" s="7"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+      <c r="S64" s="2"/>
+      <c r="T64" s="2"/>
+      <c r="U64" s="2"/>
+      <c r="W64"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B65" s="14"/>
       <c r="C65" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H65" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="H65" s="2"/>
       <c r="I65" s="7"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="7"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -4912,67 +5136,67 @@
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
-      <c r="U65" s="3"/>
-      <c r="V65"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U65" s="2"/>
+      <c r="V65" s="3"/>
+      <c r="W65"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H66" s="2"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A67" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E66" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F66" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-      <c r="S66" s="2"/>
-      <c r="T66" s="2"/>
-      <c r="V66"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A67" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="2"/>
+      <c r="F67" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
@@ -4983,32 +5207,33 @@
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
-      <c r="U67" s="3"/>
-      <c r="V67"/>
-    </row>
-    <row r="68" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="B68" s="30"/>
+      <c r="U67" s="2"/>
+      <c r="V67" s="3"/>
+      <c r="W67"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A68" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="14"/>
       <c r="C68" s="23" t="s">
-        <v>173</v>
+        <v>86</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H68" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="H68" s="2"/>
       <c r="I68" s="7"/>
-      <c r="J68" s="2"/>
+      <c r="J68" s="7"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -5016,11 +5241,85 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
-      <c r="R68" s="32"/>
-      <c r="S68" s="32"/>
-      <c r="T68" s="32"/>
-      <c r="U68" s="3"/>
-      <c r="V68"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="W68"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A69" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H69" s="4"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="3"/>
+      <c r="W69"/>
+    </row>
+    <row r="70" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="29"/>
+      <c r="C70" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2"/>
+      <c r="S70" s="31"/>
+      <c r="T70" s="31"/>
+      <c r="U70" s="31"/>
+      <c r="V70" s="3"/>
+      <c r="W70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5049,100 +5348,100 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>231</v>
+        <v>185</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>252</v>
+        <v>241</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>242</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>256</v>
+        <v>244</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>257</v>
+        <v>243</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>247</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>210</v>
-      </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>258</v>
+        <v>245</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>248</v>
       </c>
       <c r="C7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin zStat update: adjust for NoData
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -1269,44 +1269,6 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1815,6 +1777,44 @@
           <color indexed="64"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2156,22 +2156,22 @@
     <tableColumn id="2" name="Raw Units" dataDxfId="20"/>
     <tableColumn id="3" name="Final Units" dataDxfId="19"/>
     <tableColumn id="6" name="Layer Classification" dataDxfId="18"/>
-    <tableColumn id="21" name="Loaded to Web System" dataDxfId="0"/>
-    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="17"/>
-    <tableColumn id="19" name="Local" dataDxfId="16"/>
-    <tableColumn id="20" name="Upstream" dataDxfId="15"/>
-    <tableColumn id="10" name="CT" dataDxfId="14"/>
-    <tableColumn id="11" name="DC" dataDxfId="13"/>
-    <tableColumn id="8" name="DE" dataDxfId="12"/>
-    <tableColumn id="12" name="MA" dataDxfId="11"/>
-    <tableColumn id="7" name="MD" dataDxfId="10"/>
-    <tableColumn id="13" name="ME" dataDxfId="9"/>
-    <tableColumn id="14" name="NJ" dataDxfId="8"/>
-    <tableColumn id="15" name="NY" dataDxfId="7"/>
-    <tableColumn id="24" name="PA" dataDxfId="6"/>
-    <tableColumn id="23" name="VA" dataDxfId="5"/>
-    <tableColumn id="17" name="VT" dataDxfId="4"/>
-    <tableColumn id="16" name="WV" dataDxfId="3"/>
+    <tableColumn id="21" name="Loaded to Web System" dataDxfId="17"/>
+    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="16"/>
+    <tableColumn id="19" name="Local" dataDxfId="15"/>
+    <tableColumn id="20" name="Upstream" dataDxfId="14"/>
+    <tableColumn id="10" name="CT" dataDxfId="13"/>
+    <tableColumn id="11" name="DC" dataDxfId="12"/>
+    <tableColumn id="8" name="DE" dataDxfId="11"/>
+    <tableColumn id="12" name="MA" dataDxfId="10"/>
+    <tableColumn id="7" name="MD" dataDxfId="9"/>
+    <tableColumn id="13" name="ME" dataDxfId="8"/>
+    <tableColumn id="14" name="NJ" dataDxfId="7"/>
+    <tableColumn id="15" name="NY" dataDxfId="6"/>
+    <tableColumn id="24" name="PA" dataDxfId="5"/>
+    <tableColumn id="23" name="VA" dataDxfId="4"/>
+    <tableColumn id="17" name="VT" dataDxfId="3"/>
+    <tableColumn id="16" name="WV" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2181,8 +2181,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E7" totalsRowShown="0">
   <autoFilter ref="A1:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Data Source" dataDxfId="2"/>
-    <tableColumn id="2" name="Data Source Description" dataDxfId="1"/>
+    <tableColumn id="1" name="Data Source" dataDxfId="1"/>
+    <tableColumn id="2" name="Data Source Description" dataDxfId="0"/>
     <tableColumn id="4" name="Raw Data Layer"/>
     <tableColumn id="5" name="URL"/>
     <tableColumn id="3" name="Data Source File Path"/>
@@ -2484,17 +2484,17 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z7" sqref="Z7"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="69.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="49" style="19" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="19" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" style="10" customWidth="1"/>
     <col min="5" max="5" width="86" style="19" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" style="19" customWidth="1"/>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="Y7"/>
     </row>
-    <row r="8" spans="1:25" ht="116.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>196</v>
       </c>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="Y13"/>
     </row>
-    <row r="14" spans="1:25" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="186" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>233</v>
       </c>
@@ -4418,7 +4418,7 @@
       <c r="W26" s="38"/>
       <c r="X26" s="38"/>
     </row>
-    <row r="27" spans="1:25" ht="348.75" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" ht="395.25" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>14</v>
       </c>
@@ -4845,7 +4845,7 @@
       <c r="W36" s="3"/>
       <c r="Y36"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>65</v>
       </c>
@@ -5580,7 +5580,7 @@
       <c r="W55" s="3"/>
       <c r="Y55"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
         <v>73</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="X57" s="3"/>
       <c r="Y57"/>
     </row>
-    <row r="58" spans="1:25" ht="93" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:25" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>42</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="W58" s="3"/>
       <c r="Y58"/>
     </row>
-    <row r="59" spans="1:25" ht="93" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>43</v>
       </c>
@@ -5812,7 +5812,7 @@
       <c r="W61" s="2"/>
       <c r="Y61"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A62" s="14" t="s">
         <v>33</v>
       </c>
@@ -5851,7 +5851,7 @@
       <c r="X62" s="3"/>
       <c r="Y62"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
update READMEs and gis scripts for fws & nlcd layers
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -1141,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,6 +1263,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2487,7 +2488,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -4611,6 +4612,7 @@
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
+      <c r="X30" s="45"/>
       <c r="Y30"/>
     </row>
     <row r="31" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
@@ -4727,6 +4729,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
+      <c r="X33" s="45"/>
       <c r="Y33"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
@@ -4843,6 +4846,7 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
+      <c r="X36" s="45"/>
       <c r="Y36"/>
     </row>
     <row r="37" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
@@ -4959,6 +4963,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
+      <c r="X39" s="45"/>
       <c r="Y39"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
@@ -5075,6 +5080,7 @@
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
+      <c r="X42" s="45"/>
       <c r="Y42"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
@@ -5191,6 +5197,7 @@
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
+      <c r="X45" s="45"/>
       <c r="Y45"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
@@ -5307,6 +5314,7 @@
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
+      <c r="X48" s="45"/>
       <c r="Y48"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.35">
@@ -5462,6 +5470,7 @@
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
+      <c r="X52" s="45"/>
       <c r="Y52"/>
     </row>
     <row r="53" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -5578,6 +5587,7 @@
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
+      <c r="X55" s="45"/>
       <c r="Y55"/>
     </row>
     <row r="56" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
@@ -5658,7 +5668,7 @@
       <c r="X57" s="3"/>
       <c r="Y57"/>
     </row>
-    <row r="58" spans="1:25" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:25" ht="93" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>42</v>
       </c>
@@ -5694,9 +5704,10 @@
       <c r="U58" s="3"/>
       <c r="V58" s="3"/>
       <c r="W58" s="3"/>
+      <c r="X58" s="45"/>
       <c r="Y58"/>
     </row>
-    <row r="59" spans="1:25" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" ht="93" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>43</v>
       </c>
@@ -5810,6 +5821,7 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
+      <c r="X61" s="45"/>
       <c r="Y61"/>
     </row>
     <row r="62" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
@@ -5887,6 +5899,7 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
+      <c r="X63" s="45"/>
       <c r="Y63"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.35">
@@ -6039,6 +6052,7 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
+      <c r="X67" s="45"/>
       <c r="Y67"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Checked all README files in basinChars sub-folders for errors
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="362">
   <si>
     <t>forest</t>
   </si>
@@ -1289,6 +1289,33 @@
   </si>
   <si>
     <t>1:12,000 to 1:63,367</t>
+  </si>
+  <si>
+    <t>TNC Dams dataset snapped to high res flowlines (Umass Land Eco Lab)</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 1</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 2</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 3</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 4</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 5</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 6</t>
+  </si>
+  <si>
+    <t>The number of dams in the contributing drainage area of degree barrier 7</t>
+  </si>
+  <si>
+    <t>The total number of dams in the contributing drainage area</t>
   </si>
 </sst>
 </file>
@@ -1415,18 +1442,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -1502,7 +1523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1565,15 +1586,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1601,13 +1617,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1619,9 +1629,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1632,211 +1639,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3200,6 +3014,166 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3509,6 +3483,46 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -3704,80 +3718,80 @@
     <tableColumn id="9" name="Description" dataDxfId="63"/>
     <tableColumn id="18" name="Name" dataDxfId="62"/>
     <tableColumn id="5" name="Data Source" dataDxfId="61"/>
-    <tableColumn id="25" name="Source Resolution" dataDxfId="4"/>
-    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="60"/>
-    <tableColumn id="2" name="Raw Units" dataDxfId="59"/>
-    <tableColumn id="22" name="Conversion Factor" dataDxfId="58"/>
-    <tableColumn id="3" name="Final Units" dataDxfId="57"/>
-    <tableColumn id="6" name="Layer Classification" dataDxfId="56"/>
-    <tableColumn id="21" name="Loaded to Web System" dataDxfId="55"/>
-    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="54"/>
-    <tableColumn id="19" name="Local" dataDxfId="53"/>
-    <tableColumn id="20" name="Upstream" dataDxfId="52"/>
-    <tableColumn id="27" name="High Res Delineation Range" dataDxfId="2"/>
-    <tableColumn id="26" name="50 ft Riparian Buffers (HRD Range)" dataDxfId="3"/>
-    <tableColumn id="29" name="100 ft Riparian Buffers (HRD Range)" dataDxfId="0"/>
-    <tableColumn id="28" name="200 ft Riparian Buffers (HRD Range)" dataDxfId="1"/>
-    <tableColumn id="10" name="CT" dataDxfId="51"/>
-    <tableColumn id="11" name="DC" dataDxfId="50"/>
-    <tableColumn id="8" name="DE" dataDxfId="49"/>
-    <tableColumn id="12" name="MA" dataDxfId="48"/>
-    <tableColumn id="7" name="MD" dataDxfId="47"/>
-    <tableColumn id="13" name="ME" dataDxfId="46"/>
-    <tableColumn id="14" name="NJ" dataDxfId="45"/>
-    <tableColumn id="15" name="NY" dataDxfId="44"/>
-    <tableColumn id="24" name="PA" dataDxfId="43"/>
-    <tableColumn id="23" name="VA" dataDxfId="42"/>
-    <tableColumn id="17" name="VT" dataDxfId="41"/>
-    <tableColumn id="16" name="WV" dataDxfId="40"/>
+    <tableColumn id="25" name="Source Resolution" dataDxfId="60"/>
+    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="59"/>
+    <tableColumn id="2" name="Raw Units" dataDxfId="58"/>
+    <tableColumn id="22" name="Conversion Factor" dataDxfId="57"/>
+    <tableColumn id="3" name="Final Units" dataDxfId="56"/>
+    <tableColumn id="6" name="Layer Classification" dataDxfId="55"/>
+    <tableColumn id="21" name="Loaded to Web System" dataDxfId="54"/>
+    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="53"/>
+    <tableColumn id="19" name="Local" dataDxfId="52"/>
+    <tableColumn id="20" name="Upstream" dataDxfId="51"/>
+    <tableColumn id="27" name="High Res Delineation Range" dataDxfId="50"/>
+    <tableColumn id="26" name="50 ft Riparian Buffers (HRD Range)" dataDxfId="49"/>
+    <tableColumn id="29" name="100 ft Riparian Buffers (HRD Range)" dataDxfId="48"/>
+    <tableColumn id="28" name="200 ft Riparian Buffers (HRD Range)" dataDxfId="47"/>
+    <tableColumn id="10" name="CT" dataDxfId="46"/>
+    <tableColumn id="11" name="DC" dataDxfId="45"/>
+    <tableColumn id="8" name="DE" dataDxfId="44"/>
+    <tableColumn id="12" name="MA" dataDxfId="43"/>
+    <tableColumn id="7" name="MD" dataDxfId="42"/>
+    <tableColumn id="13" name="ME" dataDxfId="41"/>
+    <tableColumn id="14" name="NJ" dataDxfId="40"/>
+    <tableColumn id="15" name="NY" dataDxfId="39"/>
+    <tableColumn id="24" name="PA" dataDxfId="38"/>
+    <tableColumn id="23" name="VA" dataDxfId="37"/>
+    <tableColumn id="17" name="VT" dataDxfId="36"/>
+    <tableColumn id="16" name="WV" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:X5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:X5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
   <autoFilter ref="A1:X5"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="Data Layer" dataDxfId="35"/>
-    <tableColumn id="9" name="Description" dataDxfId="34"/>
-    <tableColumn id="18" name="Name" dataDxfId="33"/>
-    <tableColumn id="5" name="Data Source" dataDxfId="32"/>
-    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="31"/>
-    <tableColumn id="2" name="Raw Units" dataDxfId="30"/>
-    <tableColumn id="3" name="Final Units" dataDxfId="29"/>
-    <tableColumn id="6" name="Layer Classification" dataDxfId="28"/>
-    <tableColumn id="21" name="Loaded to Web System" dataDxfId="27"/>
-    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="26"/>
-    <tableColumn id="19" name="Local" dataDxfId="25"/>
-    <tableColumn id="20" name="Upstream" dataDxfId="24"/>
-    <tableColumn id="10" name="CT" dataDxfId="23"/>
-    <tableColumn id="11" name="DC" dataDxfId="22"/>
-    <tableColumn id="8" name="DE" dataDxfId="21"/>
-    <tableColumn id="12" name="MA" dataDxfId="20"/>
-    <tableColumn id="7" name="MD" dataDxfId="19"/>
-    <tableColumn id="13" name="ME" dataDxfId="18"/>
-    <tableColumn id="14" name="NJ" dataDxfId="17"/>
-    <tableColumn id="15" name="NY" dataDxfId="16"/>
-    <tableColumn id="24" name="PA" dataDxfId="15"/>
-    <tableColumn id="23" name="VA" dataDxfId="14"/>
-    <tableColumn id="17" name="VT" dataDxfId="13"/>
-    <tableColumn id="16" name="WV" dataDxfId="12"/>
+    <tableColumn id="1" name="Data Layer" dataDxfId="30"/>
+    <tableColumn id="9" name="Description" dataDxfId="29"/>
+    <tableColumn id="18" name="Name" dataDxfId="28"/>
+    <tableColumn id="5" name="Data Source" dataDxfId="27"/>
+    <tableColumn id="47" name="Layer Development GitHub Repo" dataDxfId="26"/>
+    <tableColumn id="2" name="Raw Units" dataDxfId="25"/>
+    <tableColumn id="3" name="Final Units" dataDxfId="24"/>
+    <tableColumn id="6" name="Layer Classification" dataDxfId="23"/>
+    <tableColumn id="21" name="Loaded to Web System" dataDxfId="22"/>
+    <tableColumn id="4" name="Automated Raster Prep" dataDxfId="21"/>
+    <tableColumn id="19" name="Local" dataDxfId="20"/>
+    <tableColumn id="20" name="Upstream" dataDxfId="19"/>
+    <tableColumn id="10" name="CT" dataDxfId="18"/>
+    <tableColumn id="11" name="DC" dataDxfId="17"/>
+    <tableColumn id="8" name="DE" dataDxfId="16"/>
+    <tableColumn id="12" name="MA" dataDxfId="15"/>
+    <tableColumn id="7" name="MD" dataDxfId="14"/>
+    <tableColumn id="13" name="ME" dataDxfId="13"/>
+    <tableColumn id="14" name="NJ" dataDxfId="12"/>
+    <tableColumn id="15" name="NY" dataDxfId="11"/>
+    <tableColumn id="24" name="PA" dataDxfId="10"/>
+    <tableColumn id="23" name="VA" dataDxfId="9"/>
+    <tableColumn id="17" name="VT" dataDxfId="8"/>
+    <tableColumn id="16" name="WV" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F11" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F11" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Data Source" dataDxfId="10"/>
-    <tableColumn id="2" name="Data Source Description" dataDxfId="9"/>
-    <tableColumn id="4" name="Raw Data Layer" dataDxfId="8"/>
-    <tableColumn id="5" name="URL" dataDxfId="7"/>
-    <tableColumn id="6" name="Citation" dataDxfId="6"/>
-    <tableColumn id="3" name="Local Data Storage File Path" dataDxfId="5"/>
+    <tableColumn id="1" name="Data Source" dataDxfId="5"/>
+    <tableColumn id="2" name="Data Source Description" dataDxfId="4"/>
+    <tableColumn id="4" name="Raw Data Layer" dataDxfId="3"/>
+    <tableColumn id="5" name="URL" dataDxfId="2"/>
+    <tableColumn id="6" name="Citation" dataDxfId="1"/>
+    <tableColumn id="3" name="Local Data Storage File Path" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4076,10 +4090,10 @@
   <dimension ref="A1:AE64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -4252,9 +4266,15 @@
       <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S2" s="2" t="s">
         <v>79</v>
       </c>
@@ -4339,9 +4359,15 @@
       <c r="O3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S3" s="2" t="s">
         <v>79</v>
       </c>
@@ -4426,9 +4452,15 @@
       <c r="O4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S4" s="2" t="s">
         <v>79</v>
       </c>
@@ -4513,9 +4545,15 @@
       <c r="O5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S5" s="2" t="s">
         <v>79</v>
       </c>
@@ -4600,9 +4638,15 @@
       <c r="O6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S6" s="2" t="s">
         <v>79</v>
       </c>
@@ -4687,9 +4731,15 @@
       <c r="O7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S7" s="2" t="s">
         <v>79</v>
       </c>
@@ -4774,9 +4824,15 @@
       <c r="O8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S8" s="2" t="s">
         <v>79</v>
       </c>
@@ -4825,10 +4881,10 @@
       <c r="C9" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="29" t="s">
         <v>342</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -4861,9 +4917,15 @@
       <c r="O9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S9" s="2" t="s">
         <v>79</v>
       </c>
@@ -4912,10 +4974,10 @@
       <c r="C10" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="29" t="s">
         <v>343</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -4948,21 +5010,51 @@
       <c r="O10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
+      <c r="P10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE10"/>
     </row>
     <row r="11" spans="1:31" ht="93" x14ac:dyDescent="0.35">
@@ -4975,10 +5067,10 @@
       <c r="C11" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="29" t="s">
         <v>343</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -5011,21 +5103,51 @@
       <c r="O11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="28"/>
+      <c r="P11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE11"/>
     </row>
     <row r="12" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -5074,21 +5196,51 @@
       <c r="O12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="28"/>
+      <c r="P12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE12"/>
     </row>
     <row r="13" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -5137,21 +5289,51 @@
       <c r="O13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="28"/>
+      <c r="P13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE13"/>
     </row>
     <row r="14" spans="1:31" ht="93" x14ac:dyDescent="0.35">
@@ -5200,21 +5382,51 @@
       <c r="O14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="P14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE14"/>
     </row>
     <row r="15" spans="1:31" ht="139.5" x14ac:dyDescent="0.35">
@@ -5224,7 +5436,7 @@
       <c r="B15" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>135</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -5251,7 +5463,7 @@
       <c r="K15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="30" t="s">
         <v>34</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -5263,9 +5475,15 @@
       <c r="O15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="P15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S15" s="2" t="s">
         <v>79</v>
       </c>
@@ -5311,7 +5529,7 @@
       <c r="B16" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>139</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -5350,9 +5568,15 @@
       <c r="O16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="P16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S16" s="2" t="s">
         <v>79</v>
       </c>
@@ -5398,7 +5622,7 @@
       <c r="B17" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>137</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -5437,9 +5661,15 @@
       <c r="O17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="P17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S17" s="2" t="s">
         <v>79</v>
       </c>
@@ -5485,7 +5715,7 @@
       <c r="B18" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>138</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -5524,9 +5754,15 @@
       <c r="O18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="P18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S18" s="2" t="s">
         <v>79</v>
       </c>
@@ -5572,7 +5808,7 @@
       <c r="B19" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>136</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -5611,9 +5847,15 @@
       <c r="O19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="P19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S19" s="2" t="s">
         <v>79</v>
       </c>
@@ -5659,7 +5901,7 @@
       <c r="B20" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>129</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -5698,9 +5940,15 @@
       <c r="O20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="P20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S20" s="2" t="s">
         <v>79</v>
       </c>
@@ -5785,9 +6033,15 @@
       <c r="O21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="P21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S21" s="2" t="s">
         <v>79</v>
       </c>
@@ -5833,7 +6087,7 @@
       <c r="B22" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>131</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -5872,9 +6126,15 @@
       <c r="O22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="P22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S22" s="2" t="s">
         <v>79</v>
       </c>
@@ -5920,7 +6180,7 @@
       <c r="B23" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -5959,9 +6219,15 @@
       <c r="O23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
+      <c r="P23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S23" s="2" t="s">
         <v>79</v>
       </c>
@@ -6007,7 +6273,7 @@
       <c r="B24" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>133</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -6046,9 +6312,15 @@
       <c r="O24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
+      <c r="P24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S24" s="2" t="s">
         <v>79</v>
       </c>
@@ -6093,7 +6365,7 @@
       <c r="B25" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>144</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -6132,9 +6404,15 @@
       <c r="O25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
+      <c r="P25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S25" s="2" t="s">
         <v>79</v>
       </c>
@@ -6179,7 +6457,7 @@
       <c r="B26" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>134</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -6218,9 +6496,15 @@
       <c r="O26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
+      <c r="P26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S26" s="2" t="s">
         <v>79</v>
       </c>
@@ -6265,7 +6549,7 @@
       <c r="B27" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>141</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -6304,9 +6588,15 @@
       <c r="O27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
+      <c r="P27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S27" s="2" t="s">
         <v>79</v>
       </c>
@@ -6345,14 +6635,14 @@
       </c>
       <c r="AE27"/>
     </row>
-    <row r="28" spans="1:31" s="24" customFormat="1" ht="279" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" s="47" customFormat="1" ht="279" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>140</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -6391,9 +6681,15 @@
       <c r="O28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="P28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S28" s="2" t="s">
         <v>79</v>
       </c>
@@ -6477,21 +6773,51 @@
       <c r="O29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
+      <c r="P29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD29" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE29"/>
     </row>
     <row r="30" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6540,21 +6866,51 @@
       <c r="O30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="28"/>
+      <c r="P30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD30" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE30"/>
     </row>
     <row r="31" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6603,21 +6959,51 @@
       <c r="O31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="28"/>
+      <c r="P31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD31" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE31"/>
     </row>
     <row r="32" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6666,21 +7052,51 @@
       <c r="O32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="30"/>
+      <c r="P32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD32" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE32"/>
     </row>
     <row r="33" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6729,21 +7145,51 @@
       <c r="O33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
+      <c r="P33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD33" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE33"/>
     </row>
     <row r="34" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6792,21 +7238,51 @@
       <c r="O34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
+      <c r="P34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE34"/>
     </row>
     <row r="35" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6855,21 +7331,51 @@
       <c r="O35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="3"/>
-      <c r="AA35" s="3"/>
-      <c r="AB35" s="3"/>
-      <c r="AC35" s="3"/>
-      <c r="AD35" s="26"/>
+      <c r="P35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE35"/>
     </row>
     <row r="36" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6918,21 +7424,51 @@
       <c r="O36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="3"/>
-      <c r="AC36" s="3"/>
-      <c r="AD36" s="28"/>
+      <c r="P36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD36" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE36"/>
     </row>
     <row r="37" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -6981,21 +7517,51 @@
       <c r="O37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="3"/>
-      <c r="AC37" s="3"/>
-      <c r="AD37" s="3"/>
+      <c r="P37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD37" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE37"/>
     </row>
     <row r="38" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -7044,21 +7610,51 @@
       <c r="O38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="30"/>
+      <c r="P38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD38" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE38"/>
     </row>
     <row r="39" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -7107,21 +7703,51 @@
       <c r="O39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
+      <c r="P39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD39" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE39"/>
     </row>
     <row r="40" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -7170,21 +7796,51 @@
       <c r="O40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="30"/>
+      <c r="P40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD40" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE40"/>
     </row>
     <row r="41" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -7233,21 +7889,51 @@
       <c r="O41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-      <c r="AB41" s="3"/>
-      <c r="AC41" s="3"/>
-      <c r="AD41" s="26"/>
+      <c r="P41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD41" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE41"/>
     </row>
     <row r="42" spans="1:31" ht="69.75" x14ac:dyDescent="0.35">
@@ -7296,21 +7982,51 @@
       <c r="O42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="30"/>
+      <c r="P42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE42"/>
     </row>
     <row r="43" spans="1:31" ht="209.25" x14ac:dyDescent="0.35">
@@ -7359,21 +8075,51 @@
       <c r="O43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="3"/>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="28"/>
+      <c r="P43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD43" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE43"/>
     </row>
     <row r="44" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7422,21 +8168,51 @@
       <c r="O44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AC44" s="3"/>
-      <c r="AD44" s="3"/>
+      <c r="P44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD44" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE44"/>
     </row>
     <row r="45" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7485,21 +8261,51 @@
       <c r="O45" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="30"/>
+      <c r="P45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD45" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE45"/>
     </row>
     <row r="46" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7548,21 +8354,51 @@
       <c r="O46" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="28"/>
+      <c r="P46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD46" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE46"/>
     </row>
     <row r="47" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7611,21 +8447,51 @@
       <c r="O47" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="7"/>
-      <c r="R47" s="7"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="2"/>
-      <c r="Z47" s="2"/>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="3"/>
-      <c r="AC47" s="3"/>
-      <c r="AD47" s="3"/>
+      <c r="P47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD47" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE47"/>
     </row>
     <row r="48" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7674,21 +8540,51 @@
       <c r="O48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2"/>
-      <c r="Z48" s="2"/>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="3"/>
-      <c r="AC48" s="3"/>
-      <c r="AD48" s="30"/>
+      <c r="P48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD48" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE48"/>
     </row>
     <row r="49" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7737,21 +8633,51 @@
       <c r="O49" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2"/>
-      <c r="Z49" s="2"/>
-      <c r="AA49" s="3"/>
-      <c r="AB49" s="3"/>
-      <c r="AC49" s="3"/>
-      <c r="AD49" s="3"/>
+      <c r="P49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD49" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="AE49"/>
     </row>
     <row r="50" spans="1:31" ht="162.75" x14ac:dyDescent="0.35">
@@ -7800,9 +8726,15 @@
       <c r="O50" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
+      <c r="P50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S50" s="2" t="s">
         <v>79</v>
       </c>
@@ -7842,13 +8774,13 @@
       <c r="AE50"/>
     </row>
     <row r="51" spans="1:31" ht="93" x14ac:dyDescent="0.35">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="36" t="s">
         <v>319</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="C51" s="41" t="s">
+      <c r="C51" s="37" t="s">
         <v>321</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -7860,19 +8792,19 @@
       <c r="F51" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G51" s="44" t="s">
+      <c r="G51" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="39">
         <v>1</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J51" s="43" t="s">
+      <c r="J51" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="K51" s="45" t="s">
+      <c r="K51" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L51" s="2" t="s">
@@ -7887,9 +8819,15 @@
       <c r="O51" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P51" s="46"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="46"/>
+      <c r="P51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="S51" s="2" t="s">
         <v>79</v>
       </c>
@@ -7928,34 +8866,38 @@
       </c>
       <c r="AE51"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A52" s="39" t="s">
+    <row r="52" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A52" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="41" t="s">
+      <c r="B52" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="C52" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="D52" s="42"/>
-      <c r="E52" s="43" t="s">
+      <c r="D52" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E52" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G52" s="44" t="s">
+      <c r="G52" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="39">
         <v>1</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J52" s="43" t="s">
+      <c r="J52" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="K52" s="45" t="s">
+      <c r="K52" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L52" s="2" t="s">
@@ -7970,9 +8912,15 @@
       <c r="O52" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P52" s="43"/>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="43"/>
+      <c r="P52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R52" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S52" s="2" t="s">
         <v>79</v>
       </c>
@@ -8011,34 +8959,38 @@
       </c>
       <c r="AE52"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A53" s="39" t="s">
+    <row r="53" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A53" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="41" t="s">
+      <c r="B53" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="43" t="s">
+      <c r="D53" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E53" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G53" s="44" t="s">
+      <c r="G53" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="39">
         <v>1</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="43" t="s">
+      <c r="J53" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="K53" s="45" t="s">
+      <c r="K53" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L53" s="2" t="s">
@@ -8053,9 +9005,15 @@
       <c r="O53" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
+      <c r="P53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S53" s="2" t="s">
         <v>79</v>
       </c>
@@ -8094,34 +9052,38 @@
       </c>
       <c r="AE53"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A54" s="39" t="s">
+    <row r="54" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A54" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="41" t="s">
+      <c r="B54" s="46" t="s">
+        <v>356</v>
+      </c>
+      <c r="C54" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D54" s="42"/>
-      <c r="E54" s="43" t="s">
+      <c r="D54" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E54" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G54" s="44" t="s">
+      <c r="G54" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="39">
         <v>1</v>
       </c>
       <c r="I54" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J54" s="43" t="s">
+      <c r="J54" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="K54" s="45" t="s">
+      <c r="K54" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L54" s="2" t="s">
@@ -8136,9 +9098,15 @@
       <c r="O54" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P54" s="43"/>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="43"/>
+      <c r="P54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S54" s="2" t="s">
         <v>79</v>
       </c>
@@ -8177,34 +9145,38 @@
       </c>
       <c r="AE54"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A55" s="39" t="s">
+    <row r="55" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A55" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41" t="s">
+      <c r="B55" s="46" t="s">
+        <v>357</v>
+      </c>
+      <c r="C55" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="42"/>
-      <c r="E55" s="43" t="s">
+      <c r="D55" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E55" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G55" s="44" t="s">
+      <c r="G55" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="39">
         <v>1</v>
       </c>
       <c r="I55" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J55" s="43" t="s">
+      <c r="J55" s="38" t="s">
         <v>333</v>
       </c>
-      <c r="K55" s="45" t="s">
+      <c r="K55" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L55" s="2" t="s">
@@ -8219,9 +9191,15 @@
       <c r="O55" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="43"/>
+      <c r="P55" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S55" s="2" t="s">
         <v>79</v>
       </c>
@@ -8260,34 +9238,38 @@
       </c>
       <c r="AE55"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A56" s="39" t="s">
+    <row r="56" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A56" s="36" t="s">
         <v>307</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="41" t="s">
+      <c r="B56" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="C56" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="D56" s="42"/>
-      <c r="E56" s="43" t="s">
+      <c r="D56" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E56" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G56" s="44" t="s">
+      <c r="G56" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="39">
         <v>1</v>
       </c>
       <c r="I56" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J56" s="43" t="s">
+      <c r="J56" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="K56" s="45" t="s">
+      <c r="K56" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L56" s="2" t="s">
@@ -8302,9 +9284,15 @@
       <c r="O56" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P56" s="46"/>
-      <c r="Q56" s="46"/>
-      <c r="R56" s="46"/>
+      <c r="P56" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S56" s="2" t="s">
         <v>79</v>
       </c>
@@ -8343,34 +9331,38 @@
       </c>
       <c r="AE56"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A57" s="39" t="s">
+    <row r="57" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A57" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="41" t="s">
+      <c r="B57" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="C57" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D57" s="42"/>
-      <c r="E57" s="43" t="s">
+      <c r="D57" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E57" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G57" s="44" t="s">
+      <c r="G57" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="39">
         <v>1</v>
       </c>
       <c r="I57" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J57" s="43" t="s">
+      <c r="J57" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="K57" s="45" t="s">
+      <c r="K57" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L57" s="2" t="s">
@@ -8385,9 +9377,15 @@
       <c r="O57" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P57" s="43"/>
-      <c r="Q57" s="43"/>
-      <c r="R57" s="43"/>
+      <c r="P57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S57" s="2" t="s">
         <v>79</v>
       </c>
@@ -8426,34 +9424,38 @@
       </c>
       <c r="AE57"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A58" s="39" t="s">
+    <row r="58" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A58" s="36" t="s">
         <v>309</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="41" t="s">
+      <c r="B58" s="46" t="s">
+        <v>360</v>
+      </c>
+      <c r="C58" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="D58" s="42"/>
-      <c r="E58" s="43" t="s">
+      <c r="D58" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E58" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G58" s="44" t="s">
+      <c r="G58" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="39">
         <v>1</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J58" s="43" t="s">
+      <c r="J58" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="K58" s="45" t="s">
+      <c r="K58" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L58" s="2" t="s">
@@ -8468,9 +9470,15 @@
       <c r="O58" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P58" s="43"/>
-      <c r="Q58" s="43"/>
-      <c r="R58" s="43"/>
+      <c r="P58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S58" s="2" t="s">
         <v>79</v>
       </c>
@@ -8509,34 +9517,38 @@
       </c>
       <c r="AE58"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A59" s="39" t="s">
+    <row r="59" spans="1:31" ht="93" x14ac:dyDescent="0.35">
+      <c r="A59" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="41" t="s">
+      <c r="B59" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="C59" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="D59" s="42"/>
-      <c r="E59" s="43" t="s">
+      <c r="D59" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E59" s="38" t="s">
         <v>325</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G59" s="44" t="s">
+      <c r="G59" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H59" s="39">
         <v>1</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J59" s="43" t="s">
+      <c r="J59" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="K59" s="45" t="s">
+      <c r="K59" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L59" s="2" t="s">
@@ -8551,9 +9563,15 @@
       <c r="O59" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P59" s="43"/>
-      <c r="Q59" s="43"/>
-      <c r="R59" s="43"/>
+      <c r="P59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S59" s="2" t="s">
         <v>79</v>
       </c>
@@ -8638,9 +9656,15 @@
       <c r="O60" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2"/>
+      <c r="P60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R60" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S60" s="2" t="s">
         <v>79</v>
       </c>
@@ -8674,7 +9698,7 @@
       <c r="AC60" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AD60" s="29" t="s">
+      <c r="AD60" s="27" t="s">
         <v>79</v>
       </c>
       <c r="AE60"/>
@@ -8725,9 +9749,15 @@
       <c r="O61" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-      <c r="R61" s="2"/>
+      <c r="P61" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R61" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S61" s="2" t="s">
         <v>79</v>
       </c>
@@ -8812,9 +9842,15 @@
       <c r="O62" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
+      <c r="P62" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R62" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S62" s="2" t="s">
         <v>79</v>
       </c>
@@ -8899,9 +9935,15 @@
       <c r="O63" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
+      <c r="P63" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R63" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S63" s="2" t="s">
         <v>79</v>
       </c>
@@ -8935,7 +9977,7 @@
       <c r="AC63" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AD63" s="29" t="s">
+      <c r="AD63" s="27" t="s">
         <v>79</v>
       </c>
       <c r="AE63"/>
@@ -8986,9 +10028,15 @@
       <c r="O64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
+      <c r="P64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R64" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="S64" s="2" t="s">
         <v>79</v>
       </c>
@@ -9218,7 +10266,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="26"/>
+      <c r="X3" s="25"/>
       <c r="Y3"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
@@ -9334,19 +10382,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="31" t="s">
         <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="31" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -9354,19 +10402,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="32" t="s">
         <v>290</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -9374,19 +10422,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="31" t="s">
         <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="32" t="s">
         <v>294</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -9394,19 +10442,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="31" t="s">
         <v>126</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="32" t="s">
         <v>292</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -9414,10 +10462,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="31" t="s">
         <v>242</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -9426,7 +10474,7 @@
       <c r="D6" t="s">
         <v>243</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="33" t="s">
         <v>241</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -9434,19 +10482,19 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="31" t="s">
         <v>246</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="33" t="s">
         <v>295</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -9454,37 +10502,37 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>275</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="33" t="s">
         <v>296</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="31" t="s">
         <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="35" t="s">
         <v>297</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -9492,35 +10540,35 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48" t="s">
+      <c r="B10" s="41"/>
+      <c r="C10" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="48"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="31" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="37"/>
+      <c r="E13" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add variable description column to documentation spreadsheet
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="367">
   <si>
     <t>forest</t>
   </si>
@@ -313,18 +313,6 @@
     <t>The average elevation across the basin.</t>
   </si>
   <si>
-    <t>The percentage of the contributing drainage area that is classified as "wetland".</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is the geologic classification "surficially coarse".</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is made up of only water bodies that do not intersect with the high resolution stream netowork.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is made up of only water bodies that intersect with the high resolution stream netowork.</t>
-  </si>
-  <si>
     <t>Raw Data Layer</t>
   </si>
   <si>
@@ -347,21 +335,6 @@
   </si>
   <si>
     <t>/Conte-Ecology/basinCharacteristics/impoundedArea</t>
-  </si>
-  <si>
-    <t>The HUC4 code associated with the centroid of the catchment</t>
-  </si>
-  <si>
-    <t>The HUC6 code associated with the centroid of the catchment</t>
-  </si>
-  <si>
-    <t>The HUC8 code associated with the centroid of the catchment</t>
-  </si>
-  <si>
-    <t>The HUC10 code associated with the centroid of the catchment</t>
-  </si>
-  <si>
-    <t>The HUC12 code associated with the centroid of the catchment</t>
   </si>
   <si>
     <t>/Conte-Ecology/basinCharacteristics/hucs</t>
@@ -483,45 +456,6 @@
 "Other"</t>
   </si>
   <si>
-    <t>The percentage of the contributing drainage area that is classified as being agricultural land.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as primarily herbacous coverage.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as open water such as lakes and ponds.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as any type of wetland.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as being covered by mixed types of forest.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as being evergreen forest.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as deciduous forest.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as developed land that is open space.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as medium intensity developmed land.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as low intensity developed land.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as high intensity developed land.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as forested land without development.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that has been developed.</t>
-  </si>
-  <si>
     <t>/Conte-Ecology/basinCharacteristics/nlcdImpervious</t>
   </si>
   <si>
@@ -546,13 +480,7 @@
     <t>fwsopenwater</t>
   </si>
   <si>
-    <t>The percentage of the contributing drainage area that is classified as "open water".</t>
-  </si>
-  <si>
     <t>Percent Sandy</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as having "sandy" soil.</t>
   </si>
   <si>
     <t>impervious</t>
@@ -635,66 +563,6 @@
 "A/D", "B/D", "C/D", or "D"</t>
   </si>
   <si>
-    <t>The average value over the contributing drainage area of the numerical translation of the 7 drainage class categories (values 1-7).</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as soil hydrologic group A.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as soil hydrologic group A or B.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as soil hydrologic group C or D.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as soil hydrologic group D only.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is any calssification containing soil hydrologic group D.</t>
-  </si>
-  <si>
-    <t>Average annual maximum temperature (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average annual minimum temperature (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average January precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average February precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average March precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average April precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average May precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average June precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average July precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average August precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average September precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average October precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average November precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>Average December precipitaiton (1981 - 2010) in the contributing drainage area.</t>
-  </si>
-  <si>
     <t>ann_tmax_c</t>
   </si>
   <si>
@@ -746,9 +614,6 @@
     <t>/Conte-Ecology/basinCharacteristics/prism</t>
   </si>
   <si>
-    <t>The average slope of the terrain in the contributing drainage area.</t>
-  </si>
-  <si>
     <t>slope_pcnt</t>
   </si>
   <si>
@@ -762,15 +627,6 @@
   </si>
   <si>
     <t>/Conte-Ecology/basinCharacteristics/atmosphericDeposition</t>
-  </si>
-  <si>
-    <t>The total wet atmoshpheric deposition of sulfate in 2011 averaged over the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>The total wet atmoshpheric deposition of nitrate in 2011 averaged over the contributing drainage area.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is classified as forest.</t>
   </si>
   <si>
     <t>Local Data Storage File Path</t>
@@ -931,9 +787,6 @@
     <t>elevation</t>
   </si>
   <si>
-    <t>The average elevation of the terrain in the contributing drainage area.</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -964,12 +817,6 @@
     <t xml:space="preserve">"WETLAND_TYPE" = 
 "Freshwater Pond", or 
 "Lake", </t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is made up of only open water bodies that do not intersect with the high resolution stream netowork.</t>
-  </si>
-  <si>
-    <t>The percentage of the contributing drainage area that is made up of only open water bodies that intersect with the high resolution stream netowork.</t>
   </si>
   <si>
     <t>Fish &amp; Wildlife Service (FWS) Nat ional Wetlands Inventory</t>
@@ -1214,9 +1061,6 @@
     <t>Spatial Polygons</t>
   </si>
   <si>
-    <t>The vertical projection of the percentage of the contributing drainage area that is covered by tree canopy.</t>
-  </si>
-  <si>
     <t>Spatial points</t>
   </si>
   <si>
@@ -1295,30 +1139,6 @@
     <t>TNC Dams dataset snapped to high res flowlines (Umass Land Eco Lab)</t>
   </si>
   <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 1</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 2</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 3</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 4</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 5</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 6</t>
-  </si>
-  <si>
-    <t>The number of dams in the contributing drainage area of degree barrier 7</t>
-  </si>
-  <si>
-    <t>The total number of dams in the contributing drainage area</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -1335,13 +1155,190 @@
   </si>
   <si>
     <t>Human Impacts</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in April spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The total wet atmoshpheric deposition of nitrate ion in 2011 spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The total wet atmoshpheric deposition of sulfate ion in 2011 spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in August spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in December spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in February spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in January spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in July spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in June spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in March spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in May spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in November spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in October spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) mean monthly precipitation in September spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) average annual maximum temperature spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The 30-year (1981 - 2010) average annual minimum temperature spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The landscape elevation spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The slope of the landscape spatially averaged over the catchment area.</t>
+  </si>
+  <si>
+    <t>The HUC10 code associated with the centroid of the catchment.</t>
+  </si>
+  <si>
+    <t>The HUC12 code associated with the centroid of the catchment.</t>
+  </si>
+  <si>
+    <t>The HUC4 code associated with the centroid of the catchment.</t>
+  </si>
+  <si>
+    <t>The HUC6 code associated with the centroid of the catchment.</t>
+  </si>
+  <si>
+    <t>The HUC8 code associated with the centroid of the catchment.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by lakes or ponds that intersect the high resolution stream netowork.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by lakes or ponds that do not intersect the high resolution stream netowork.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by wetlands, lakes, or ponds that do not intersect the high resolution stream netowork.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by wetlands, lakes, or ponds that intersect the high resolution stream netowork.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by agricultural land (e.g. cultivated crops, orchards, and pasture) including fallow land.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area covered by places where people work or live in high numbers. These areas are typically covered by more than 80% impervious surface.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by areas with a mixture of vegetation and constructed materials, such as single family housing units. These areas are typically covered by 20% - 49% impervious surface.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by areas with a mixture of vegetation and constructed materials, such as single family housing units. These areas are typically covered by 50% - 79% impervious surface.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by some constructed materials, but mostly lawn grass vegetation such as parks, golf courses, and single family housing units on large lots. These areas are typically covered by less than 20% impervious surface.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that has been developed by human activity to any extent.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is dominated by herbaceous vegetation not intensively managed.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by trees taller than 5 meters and dominated by species that lose their foliage in repsonse to season change.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by trees taller than 5 meters and dominated by species that maintain foliage year-round.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area made up of any trees taller than 5 meters.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by trees taller than 5 meters and not dominated by either evergreen or deciduous.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment areacovered by ponds, lakes, or deep estuary/marine water.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area covered by open water.</t>
+  </si>
+  <si>
+    <t>The vertical projection of the percentage of the catchment area that is covered by tree canopy.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is classified as forested land with developed land treated as missing data. This layer serves as an attempt to avoid high correlation between forested and impervious surface in the northeastern U.S.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is classified as any type of wetland.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by a perent soil material with texture described as "sandy".</t>
+  </si>
+  <si>
+    <t>The numerical average of the rank of seven drainage class categories over the catchment area. These categories describe the natural drainage conditions of the soil referring to frequency and duration of wet periods. Values range from 1 (Excessively drained) to 7 (Very poorly drained).</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area with soil classified as hydrologic group D. These soils have high runoff potential and very low infiltration and water transmission rates.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area with soil classified as hydrologic groups C or D. These soils have low to very low infiltration and water transmission rates.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area with soil classified as hydrologic groups A or B. These soils have moderate to high infiltration and water transmission rates.</t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area with soil classified as hydrologic group A. These soils have a low runoff potential and high infiltration and water transmission rates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of the catchment area with soil classified as hydrologic group D, including soils described as group A, B, or C but have a high water table putting them in the D group. These soils have high runoff potential and very low infiltration and water transmission rates. </t>
+  </si>
+  <si>
+    <t>The percentage of the catchment area that is covered by a perent soil material with texture described as "sandy", "gravelly", or a combination of the two.</t>
+  </si>
+  <si>
+    <t>The total number of dams in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number of partially breached dams in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number of small dam barriers (1 - 12 feet) in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number of complete barriers to all fish (greater than 12 feet) in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number of barriers with a fish ladder in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number fully breached, unlikely barriers in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number unknown, but assumd full barriers in the catchment area.</t>
+  </si>
+  <si>
+    <t>The number of locks in the catchment area.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1460,6 +1457,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1539,10 +1544,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1613,9 +1619,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1641,9 +1644,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1667,11 +1667,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="105">
@@ -2752,13 +2751,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
@@ -2772,6 +2764,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4989,7 +4988,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
   <autoFilter ref="A1:AE2"/>
   <sortState ref="A2:AE64">
     <sortCondition ref="A1:A64"/>
@@ -5327,15 +5326,16 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="69.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="49" style="18" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" style="18" customWidth="1"/>
     <col min="3" max="4" width="25.5703125" style="18" customWidth="1"/>
-    <col min="5" max="6" width="31.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="42" style="10" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" style="10" customWidth="1"/>
     <col min="7" max="7" width="92.5703125" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="18" customWidth="1"/>
@@ -5373,22 +5373,22 @@
         <v>77</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>362</v>
+        <v>302</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>64</v>
@@ -5397,10 +5397,10 @@
         <v>96</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>88</v>
@@ -5409,16 +5409,16 @@
         <v>89</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>337</v>
+        <v>285</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>338</v>
+        <v>286</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>340</v>
+        <v>288</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>4</v>
@@ -5457,27 +5457,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>236</v>
+        <v>309</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>285</v>
+        <v>234</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>343</v>
+        <v>291</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>234</v>
+        <v>189</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>23</v>
@@ -5492,7 +5492,7 @@
         <v>90</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>34</v>
@@ -5553,27 +5553,27 @@
       </c>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>235</v>
+        <v>310</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>285</v>
+        <v>234</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>343</v>
+        <v>291</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>234</v>
+        <v>189</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>23</v>
@@ -5588,7 +5588,7 @@
         <v>90</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>34</v>
@@ -5654,22 +5654,22 @@
         <v>38</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>203</v>
+        <v>308</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>16</v>
@@ -5683,8 +5683,8 @@
       <c r="K4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>52</v>
+      <c r="L4" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>34</v>
@@ -5750,22 +5750,22 @@
         <v>42</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>207</v>
+        <v>311</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>16</v>
@@ -5779,8 +5779,8 @@
       <c r="K5" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>52</v>
+      <c r="L5" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>34</v>
@@ -5846,22 +5846,22 @@
         <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>211</v>
+        <v>312</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>16</v>
@@ -5875,8 +5875,8 @@
       <c r="K6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>52</v>
+      <c r="L6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>34</v>
@@ -5942,22 +5942,22 @@
         <v>36</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>201</v>
+        <v>313</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>16</v>
@@ -5971,8 +5971,8 @@
       <c r="K7" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>52</v>
+      <c r="L7" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>34</v>
@@ -6038,22 +6038,22 @@
         <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>200</v>
+        <v>314</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>16</v>
@@ -6067,8 +6067,8 @@
       <c r="K8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>52</v>
+      <c r="L8" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>34</v>
@@ -6133,23 +6133,23 @@
       <c r="A9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>206</v>
+      <c r="B9" s="8" t="s">
+        <v>315</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>16</v>
@@ -6163,8 +6163,8 @@
       <c r="K9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>52</v>
+      <c r="L9" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>34</v>
@@ -6229,23 +6229,23 @@
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>205</v>
+      <c r="B10" s="8" t="s">
+        <v>316</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>16</v>
@@ -6259,8 +6259,8 @@
       <c r="K10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>52</v>
+      <c r="L10" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>34</v>
@@ -6325,23 +6325,23 @@
       <c r="A11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>202</v>
+      <c r="B11" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>16</v>
@@ -6355,8 +6355,8 @@
       <c r="K11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>52</v>
+      <c r="L11" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>34</v>
@@ -6422,37 +6422,37 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>198</v>
+        <v>322</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="I12" s="16">
         <v>1</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>52</v>
+      <c r="L12" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>34</v>
@@ -6517,23 +6517,23 @@
       <c r="A13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>204</v>
+      <c r="B13" s="8" t="s">
+        <v>318</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>16</v>
@@ -6547,8 +6547,8 @@
       <c r="K13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>52</v>
+      <c r="L13" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>34</v>
@@ -6614,37 +6614,37 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>199</v>
+        <v>323</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="I14" s="16">
         <v>1</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>52</v>
+      <c r="L14" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>34</v>
@@ -6709,23 +6709,23 @@
       <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>210</v>
+      <c r="B15" s="8" t="s">
+        <v>319</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>224</v>
+        <v>180</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>16</v>
@@ -6739,8 +6739,8 @@
       <c r="K15" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>52</v>
+      <c r="L15" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>34</v>
@@ -6805,23 +6805,23 @@
       <c r="A16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>209</v>
+      <c r="B16" s="8" t="s">
+        <v>320</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>16</v>
@@ -6835,8 +6835,8 @@
       <c r="K16" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>52</v>
+      <c r="L16" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>34</v>
@@ -6902,22 +6902,22 @@
         <v>43</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>208</v>
+        <v>321</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>16</v>
@@ -6931,8 +6931,8 @@
       <c r="K17" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>52</v>
+      <c r="L17" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>34</v>
@@ -6998,37 +6998,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>286</v>
+        <v>235</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>52</v>
+      <c r="L18" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>47</v>
@@ -7091,25 +7091,25 @@
     </row>
     <row r="19" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>229</v>
+        <v>325</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>286</v>
+        <v>235</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>14</v>
@@ -7123,8 +7123,8 @@
       <c r="K19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>52</v>
+      <c r="L19" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>34</v>
@@ -7185,12 +7185,12 @@
       </c>
       <c r="AF19"/>
     </row>
-    <row r="20" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>113</v>
+        <v>326</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>68</v>
@@ -7199,28 +7199,28 @@
         <v>47</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>52</v>
+        <v>112</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>34</v>
@@ -7281,12 +7281,12 @@
       </c>
       <c r="AF20"/>
     </row>
-    <row r="21" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>114</v>
+        <v>327</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>62</v>
@@ -7295,28 +7295,28 @@
         <v>47</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>52</v>
+        <v>113</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>34</v>
@@ -7377,12 +7377,12 @@
       </c>
       <c r="AF21"/>
     </row>
-    <row r="22" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>110</v>
+        <v>328</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>60</v>
@@ -7391,28 +7391,28 @@
         <v>47</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>52</v>
+        <v>109</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>34</v>
@@ -7473,12 +7473,12 @@
       </c>
       <c r="AF22"/>
     </row>
-    <row r="23" spans="1:32" s="1" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>67</v>
@@ -7487,28 +7487,28 @@
         <v>47</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>52</v>
+        <v>110</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>34</v>
@@ -7568,12 +7568,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="1" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>112</v>
+        <v>330</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>61</v>
@@ -7582,28 +7582,28 @@
         <v>47</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I24" s="13">
         <v>1</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>52</v>
+        <v>111</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>34</v>
@@ -7663,27 +7663,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:32" s="1" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>279</v>
+        <v>230</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>63</v>
@@ -7695,9 +7695,9 @@
         <v>14</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="L25" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -7760,25 +7760,25 @@
     </row>
     <row r="26" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>277</v>
+        <v>228</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>100</v>
+        <v>333</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>63</v>
@@ -7790,9 +7790,9 @@
         <v>14</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="L26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -7854,27 +7854,27 @@
       </c>
       <c r="AF26"/>
     </row>
-    <row r="27" spans="1:32" s="45" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" s="43" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>280</v>
+        <v>231</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>63</v>
@@ -7886,9 +7886,9 @@
         <v>14</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="L27" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -7951,25 +7951,25 @@
     </row>
     <row r="28" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>278</v>
+        <v>229</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>101</v>
+        <v>334</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>63</v>
@@ -7981,9 +7981,9 @@
         <v>14</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="L28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M28" s="2" t="s">
@@ -8047,25 +8047,25 @@
     </row>
     <row r="29" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>149</v>
+        <v>335</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>63</v>
@@ -8077,9 +8077,9 @@
         <v>14</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="L29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M29" s="3" t="s">
@@ -8141,27 +8141,27 @@
       </c>
       <c r="AF29"/>
     </row>
-    <row r="30" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:32" ht="93" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>155</v>
+        <v>342</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>63</v>
@@ -8173,9 +8173,9 @@
         <v>14</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="L30" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M30" s="2" t="s">
@@ -8239,25 +8239,25 @@
     </row>
     <row r="31" spans="1:32" ht="186" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>161</v>
+        <v>340</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>63</v>
@@ -8269,9 +8269,9 @@
         <v>14</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="L31" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M31" s="2" t="s">
@@ -8333,27 +8333,27 @@
       </c>
       <c r="AF31"/>
     </row>
-    <row r="32" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>159</v>
+        <v>336</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>63</v>
@@ -8365,9 +8365,9 @@
         <v>14</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="L32" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L32" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -8429,27 +8429,27 @@
       </c>
       <c r="AF32"/>
     </row>
-    <row r="33" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>158</v>
+        <v>337</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>63</v>
@@ -8461,9 +8461,9 @@
         <v>14</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="L33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M33" s="2" t="s">
@@ -8525,27 +8525,27 @@
       </c>
       <c r="AF33"/>
     </row>
-    <row r="34" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>157</v>
+        <v>338</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>63</v>
@@ -8557,9 +8557,9 @@
         <v>14</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="L34" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L34" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M34" s="2" t="s">
@@ -8621,27 +8621,27 @@
       </c>
       <c r="AF34"/>
     </row>
-    <row r="35" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>156</v>
+        <v>339</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>63</v>
@@ -8653,9 +8653,9 @@
         <v>14</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="L35" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M35" s="2" t="s">
@@ -8722,22 +8722,22 @@
         <v>58</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>154</v>
+        <v>343</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>63</v>
@@ -8749,9 +8749,9 @@
         <v>14</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="L36" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -8818,22 +8818,22 @@
         <v>7</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>237</v>
+        <v>344</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>63</v>
@@ -8845,9 +8845,9 @@
         <v>14</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="L37" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -8911,25 +8911,25 @@
     </row>
     <row r="38" spans="1:32" ht="348.75" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>150</v>
+        <v>341</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>63</v>
@@ -8941,9 +8941,9 @@
         <v>14</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="L38" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="L38" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M38" s="3" t="s">
@@ -9005,27 +9005,27 @@
       </c>
       <c r="AF38"/>
     </row>
-    <row r="39" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>287</v>
+        <v>236</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>14</v>
@@ -9040,7 +9040,7 @@
         <v>90</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>34</v>
@@ -9106,22 +9106,22 @@
         <v>59</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>153</v>
+        <v>345</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>63</v>
@@ -9133,9 +9133,9 @@
         <v>14</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="L40" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M40" s="2" t="s">
@@ -9202,22 +9202,22 @@
         <v>10</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>169</v>
+        <v>346</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>63</v>
@@ -9229,10 +9229,10 @@
         <v>14</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>52</v>
+        <v>145</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>34</v>
@@ -9293,27 +9293,27 @@
       </c>
       <c r="AF41"/>
     </row>
-    <row r="42" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>151</v>
+        <v>347</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>63</v>
@@ -9325,9 +9325,9 @@
         <v>14</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="L42" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="L42" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M42" s="3" t="s">
@@ -9389,27 +9389,27 @@
       </c>
       <c r="AF42"/>
     </row>
-    <row r="43" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>171</v>
+        <v>351</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>351</v>
+        <v>299</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>63</v>
@@ -9421,10 +9421,10 @@
         <v>14</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>34</v>
@@ -9485,42 +9485,42 @@
       </c>
       <c r="AF43"/>
     </row>
-    <row r="44" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
-        <v>319</v>
+    <row r="44" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A44" s="33" t="s">
+        <v>268</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C44" s="47" t="s">
-        <v>321</v>
-      </c>
-      <c r="D44" s="47" t="s">
-        <v>364</v>
+        <v>348</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>304</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H44" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="H44" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I44" s="37">
+      <c r="I44" s="36">
         <v>1</v>
       </c>
       <c r="J44" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="36" t="s">
+      <c r="K44" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="L44" s="48" t="s">
-        <v>52</v>
+      <c r="L44" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>34</v>
@@ -9586,22 +9586,22 @@
         <v>8</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>160</v>
+        <v>349</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>63</v>
@@ -9613,10 +9613,10 @@
         <v>14</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>34</v>
@@ -9682,22 +9682,22 @@
         <v>9</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>98</v>
+        <v>350</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>63</v>
@@ -9709,9 +9709,9 @@
         <v>14</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="L46" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L46" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M46" s="2" t="s">
@@ -9778,22 +9778,22 @@
         <v>9</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>350</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>63</v>
@@ -9805,9 +9805,9 @@
         <v>14</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="L47" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L47" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M47" s="3" t="s">
@@ -9874,37 +9874,37 @@
         <v>28</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>192</v>
+        <v>352</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>345</v>
+        <v>293</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="I48" s="2">
         <v>1</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>34</v>
@@ -9965,27 +9965,27 @@
       </c>
       <c r="AF48"/>
     </row>
-    <row r="49" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>193</v>
+        <v>356</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>346</v>
+        <v>294</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>63</v>
@@ -9997,10 +9997,10 @@
         <v>14</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>34</v>
@@ -10061,27 +10061,27 @@
       </c>
       <c r="AF49"/>
     </row>
-    <row r="50" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>194</v>
+        <v>355</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>347</v>
+        <v>295</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>63</v>
@@ -10093,10 +10093,10 @@
         <v>14</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="L50" s="28" t="s">
-        <v>52</v>
+        <v>164</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>34</v>
@@ -10157,27 +10157,27 @@
       </c>
       <c r="AF50"/>
     </row>
-    <row r="51" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="44" t="s">
-        <v>195</v>
+      <c r="B51" s="8" t="s">
+        <v>354</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="E51" s="43" t="s">
-        <v>289</v>
+        <v>306</v>
+      </c>
+      <c r="E51" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>348</v>
+        <v>296</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>63</v>
@@ -10189,10 +10189,10 @@
         <v>14</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="L51" s="28" t="s">
-        <v>52</v>
+        <v>165</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>34</v>
@@ -10257,23 +10257,23 @@
       <c r="A52" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="44" t="s">
-        <v>197</v>
+      <c r="B52" s="8" t="s">
+        <v>357</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="E52" s="43" t="s">
-        <v>289</v>
+        <v>306</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>350</v>
+        <v>298</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="H52" s="13" t="s">
         <v>63</v>
@@ -10285,10 +10285,10 @@
         <v>14</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="L52" s="28" t="s">
-        <v>52</v>
+        <v>167</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>34</v>
@@ -10349,27 +10349,27 @@
       </c>
       <c r="AF52"/>
     </row>
-    <row r="53" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B53" s="44" t="s">
-        <v>196</v>
+      <c r="B53" s="8" t="s">
+        <v>353</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="E53" s="43" t="s">
-        <v>289</v>
+        <v>306</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>63</v>
@@ -10381,10 +10381,10 @@
         <v>14</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="L53" s="28" t="s">
-        <v>52</v>
+        <v>166</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>34</v>
@@ -10445,27 +10445,27 @@
       </c>
       <c r="AF53"/>
     </row>
-    <row r="54" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="44" t="s">
-        <v>99</v>
+      <c r="B54" s="8" t="s">
+        <v>358</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>85</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="E54" s="43" t="s">
-        <v>289</v>
+        <v>306</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>352</v>
+        <v>300</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>63</v>
@@ -10477,9 +10477,9 @@
         <v>14</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="L54" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="L54" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M54" s="2" t="s">
@@ -10541,42 +10541,42 @@
       </c>
       <c r="AF54"/>
     </row>
-    <row r="55" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A55" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>361</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>318</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>367</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="F55" s="36" t="s">
-        <v>325</v>
+    <row r="55" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A55" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="B55" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H55" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I55" s="37">
+        <v>273</v>
+      </c>
+      <c r="H55" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I55" s="36">
         <v>1</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K55" s="36" t="s">
+      <c r="K55" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="L55" s="38" t="s">
-        <v>52</v>
+      <c r="L55" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>34</v>
@@ -10637,42 +10637,42 @@
       </c>
       <c r="AF55"/>
     </row>
-    <row r="56" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A56" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>354</v>
-      </c>
-      <c r="C56" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>367</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="F56" s="36" t="s">
-        <v>325</v>
+    <row r="56" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A56" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="E56" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H56" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I56" s="37">
+        <v>273</v>
+      </c>
+      <c r="H56" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I56" s="36">
         <v>1</v>
       </c>
       <c r="J56" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K56" s="36" t="s">
-        <v>330</v>
-      </c>
-      <c r="L56" s="38" t="s">
-        <v>52</v>
+      <c r="K56" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>34</v>
@@ -10733,42 +10733,42 @@
       </c>
       <c r="AF56"/>
     </row>
-    <row r="57" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A57" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="B57" s="44" t="s">
-        <v>355</v>
-      </c>
-      <c r="C57" s="35" t="s">
-        <v>312</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>367</v>
-      </c>
-      <c r="E57" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="F57" s="36" t="s">
-        <v>325</v>
+    <row r="57" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A57" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D57" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H57" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I57" s="37">
+        <v>273</v>
+      </c>
+      <c r="H57" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I57" s="36">
         <v>1</v>
       </c>
       <c r="J57" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K57" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="L57" s="38" t="s">
-        <v>52</v>
+      <c r="K57" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>34</v>
@@ -10829,42 +10829,42 @@
       </c>
       <c r="AF57"/>
     </row>
-    <row r="58" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A58" s="34" t="s">
-        <v>305</v>
-      </c>
-      <c r="B58" s="44" t="s">
-        <v>356</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>313</v>
-      </c>
-      <c r="D58" s="46" t="s">
-        <v>367</v>
-      </c>
-      <c r="E58" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="F58" s="36" t="s">
-        <v>325</v>
+    <row r="58" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A58" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H58" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I58" s="37">
+        <v>273</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I58" s="36">
         <v>1</v>
       </c>
       <c r="J58" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K58" s="36" t="s">
-        <v>332</v>
-      </c>
-      <c r="L58" s="38" t="s">
-        <v>52</v>
+      <c r="K58" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>34</v>
@@ -10925,42 +10925,42 @@
       </c>
       <c r="AF58"/>
     </row>
-    <row r="59" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A59" s="34" t="s">
-        <v>306</v>
+    <row r="59" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A59" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>314</v>
-      </c>
-      <c r="D59" s="47" t="s">
-        <v>367</v>
+        <v>363</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>307</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F59" s="36" t="s">
-        <v>325</v>
+        <v>301</v>
+      </c>
+      <c r="F59" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H59" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I59" s="37">
+        <v>273</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I59" s="36">
         <v>1</v>
       </c>
       <c r="J59" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K59" s="36" t="s">
-        <v>333</v>
-      </c>
-      <c r="L59" s="48" t="s">
-        <v>52</v>
+      <c r="K59" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>34</v>
@@ -11021,42 +11021,42 @@
       </c>
       <c r="AF59"/>
     </row>
-    <row r="60" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A60" s="34" t="s">
+    <row r="60" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A60" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="D60" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>315</v>
-      </c>
-      <c r="D60" s="47" t="s">
-        <v>367</v>
-      </c>
       <c r="E60" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F60" s="36" t="s">
-        <v>325</v>
+        <v>301</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H60" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I60" s="37">
+        <v>273</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I60" s="36">
         <v>1</v>
       </c>
       <c r="J60" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K60" s="36" t="s">
-        <v>334</v>
-      </c>
-      <c r="L60" s="48" t="s">
-        <v>52</v>
+      <c r="K60" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M60" s="2" t="s">
         <v>34</v>
@@ -11117,42 +11117,42 @@
       </c>
       <c r="AF60"/>
     </row>
-    <row r="61" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A61" s="34" t="s">
-        <v>308</v>
+    <row r="61" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A61" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="C61" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="D61" s="47" t="s">
-        <v>367</v>
+        <v>365</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="45" t="s">
+        <v>307</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F61" s="36" t="s">
-        <v>325</v>
+        <v>301</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H61" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I61" s="37">
+        <v>273</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I61" s="36">
         <v>1</v>
       </c>
       <c r="J61" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K61" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="L61" s="48" t="s">
-        <v>52</v>
+      <c r="K61" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>34</v>
@@ -11213,42 +11213,42 @@
       </c>
       <c r="AF61"/>
     </row>
-    <row r="62" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A62" s="34" t="s">
-        <v>309</v>
+    <row r="62" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A62" s="33" t="s">
+        <v>258</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="C62" s="47" t="s">
-        <v>317</v>
-      </c>
-      <c r="D62" s="47" t="s">
-        <v>367</v>
+        <v>366</v>
+      </c>
+      <c r="C62" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="45" t="s">
+        <v>307</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F62" s="36" t="s">
-        <v>325</v>
+        <v>301</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H62" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="I62" s="37">
+        <v>273</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I62" s="36">
         <v>1</v>
       </c>
       <c r="J62" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K62" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="L62" s="48" t="s">
-        <v>52</v>
+      <c r="K62" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>34</v>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="AF62"/>
     </row>
-    <row r="63" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>25</v>
       </c>
@@ -11320,16 +11320,16 @@
         <v>78</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>24</v>
@@ -11343,7 +11343,7 @@
       <c r="K63" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="L63" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M63" s="2" t="s">
@@ -11473,10 +11473,10 @@
         <v>76</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>64</v>
@@ -11485,10 +11485,10 @@
         <v>96</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>88</v>
@@ -11678,7 +11678,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11699,32 +11699,32 @@
         <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="F1" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>103</v>
+      <c r="B2" s="28" t="s">
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -11732,179 +11732,182 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>290</v>
+      <c r="A3" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>239</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>125</v>
+      <c r="A4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>291</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>294</v>
+        <v>206</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>243</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>126</v>
+      <c r="A5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>292</v>
+        <v>206</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>241</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>242</v>
+      <c r="A6" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>194</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>241</v>
+        <v>208</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>193</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>246</v>
+      <c r="A7" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>198</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>295</v>
+        <v>208</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>244</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>275</v>
+      <c r="A8" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>296</v>
+        <v>208</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>245</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>127</v>
+      <c r="A9" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>118</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>297</v>
+        <v>206</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>246</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>329</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40" t="s">
-        <v>328</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="40"/>
+      <c r="A10" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+        <v>207</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="32"/>
+      <c r="E13" s="31"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" location="2011"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11966,22 +11969,22 @@
         <v>77</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>362</v>
+        <v>302</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>64</v>
@@ -11990,10 +11993,10 @@
         <v>96</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>88</v>
@@ -12002,16 +12005,16 @@
         <v>89</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>337</v>
+        <v>285</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>338</v>
+        <v>286</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>340</v>
+        <v>288</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>4</v>
@@ -12061,16 +12064,16 @@
         <v>19</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>86</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update scripts for NHDHRDV2
</commit_message>
<xml_diff>
--- a/Covariate Data Status - High Res Delineation.xlsx
+++ b/Covariate Data Status - High Res Delineation.xlsx
@@ -1548,7 +1548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1661,13 +1661,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4899,8 +4906,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AE63" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101">
   <autoFilter ref="A1:AE63"/>
-  <sortState ref="A2:AE64">
-    <sortCondition ref="A1:A64"/>
+  <sortState ref="A2:AE63">
+    <sortCondition ref="E1:E63"/>
   </sortState>
   <tableColumns count="31">
     <tableColumn id="1" name="Data Layer" dataDxfId="100"/>
@@ -5323,10 +5330,10 @@
   <dimension ref="A1:AF63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -5457,39 +5464,39 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="93" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>187</v>
+        <v>249</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>291</v>
+        <v>304</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>289</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="13">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="2">
+        <v>100</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>34</v>
@@ -5553,39 +5560,39 @@
       </c>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>21</v>
+        <v>228</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>291</v>
+        <v>304</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>289</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="13">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="2">
+        <v>100</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>34</v>
@@ -5651,37 +5658,37 @@
     </row>
     <row r="4" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>38</v>
+        <v>231</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="13">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="2">
+        <v>100</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>34</v>
@@ -5745,39 +5752,39 @@
       </c>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>177</v>
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="13">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="2">
+        <v>100</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>34</v>
@@ -5843,37 +5850,37 @@
     </row>
     <row r="6" spans="1:32" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>312</v>
+        <v>346</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="13">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="2">
+        <v>100</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>34</v>
@@ -5937,39 +5944,39 @@
       </c>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="93" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="13">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="2">
+        <v>100</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>34</v>
@@ -6033,45 +6040,45 @@
       </c>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>314</v>
+        <v>95</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>292</v>
+        <v>303</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="13">
+        <v>104</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2">
         <v>1</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>90</v>
+        <v>24</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>34</v>
@@ -6131,34 +6138,34 @@
     </row>
     <row r="9" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>291</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I9" s="13">
         <v>1</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>90</v>
@@ -6227,34 +6234,34 @@
     </row>
     <row r="10" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>291</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>90</v>
@@ -6323,34 +6330,34 @@
     </row>
     <row r="11" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>16</v>
+        <v>223</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>16</v>
+        <v>223</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>90</v>
@@ -6359,7 +6366,7 @@
         <v>34</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>34</v>
@@ -6419,34 +6426,34 @@
     </row>
     <row r="12" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="I12" s="16">
         <v>1</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>90</v>
@@ -6515,36 +6522,36 @@
     </row>
     <row r="13" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>318</v>
+        <v>149</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" s="16">
         <v>1</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="20" t="s">
         <v>90</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -6563,13 +6570,13 @@
         <v>34</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T13" s="2" t="s">
         <v>79</v>
@@ -6609,44 +6616,44 @@
       </c>
       <c r="AF13"/>
     </row>
-    <row r="14" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>169</v>
+        <v>335</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I14" s="16">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="4">
+        <v>100</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="49" t="s">
         <v>34</v>
       </c>
       <c r="N14" s="2" t="s">
@@ -6705,39 +6712,39 @@
       </c>
       <c r="AF14"/>
     </row>
-    <row r="15" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>45</v>
+    <row r="15" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>180</v>
+        <v>342</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>122</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="16">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="4">
+        <v>100</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>90</v>
+        <v>214</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>34</v>
@@ -6801,39 +6808,39 @@
       </c>
       <c r="AF15"/>
     </row>
-    <row r="16" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" ht="186" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>179</v>
+        <v>340</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>120</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="16">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="4">
+        <v>100</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>90</v>
+        <v>209</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>34</v>
@@ -6851,13 +6858,13 @@
         <v>34</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T16" s="2" t="s">
         <v>79</v>
@@ -6897,39 +6904,39 @@
       </c>
       <c r="AF16"/>
     </row>
-    <row r="17" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>43</v>
+    <row r="17" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>178</v>
+        <v>336</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="2">
+        <v>100</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>90</v>
+        <v>210</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>34</v>
@@ -6947,13 +6954,13 @@
         <v>34</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>79</v>
@@ -6993,45 +7000,45 @@
       </c>
       <c r="AF17"/>
     </row>
-    <row r="18" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>17</v>
+    <row r="18" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>222</v>
+        <v>337</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>290</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="I18" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="2">
+        <v>100</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>223</v>
+        <v>14</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>90</v>
+        <v>212</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>34</v>
@@ -7043,13 +7050,13 @@
         <v>34</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>79</v>
@@ -7089,39 +7096,39 @@
       </c>
       <c r="AF18"/>
     </row>
-    <row r="19" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>182</v>
+    <row r="19" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>185</v>
+        <v>338</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>129</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>290</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="2">
+        <v>100</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>34</v>
@@ -7139,13 +7146,13 @@
         <v>34</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>79</v>
@@ -7185,39 +7192,39 @@
       </c>
       <c r="AF19"/>
     </row>
-    <row r="20" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>66</v>
+    <row r="20" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>68</v>
+        <v>339</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>127</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="2">
+        <v>100</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>34</v>
@@ -7235,13 +7242,13 @@
         <v>34</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>79</v>
@@ -7281,39 +7288,39 @@
       </c>
       <c r="AF20"/>
     </row>
-    <row r="21" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>51</v>
+    <row r="21" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>62</v>
+        <v>343</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>123</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="2">
+        <v>100</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>34</v>
@@ -7377,39 +7384,39 @@
       </c>
       <c r="AF21"/>
     </row>
-    <row r="22" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I22" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="2">
+        <v>100</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>34</v>
@@ -7427,13 +7434,13 @@
         <v>34</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>79</v>
@@ -7473,44 +7480,44 @@
       </c>
       <c r="AF22"/>
     </row>
-    <row r="23" spans="1:32" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" s="1" customFormat="1" ht="348.75" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>67</v>
+        <v>341</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I23" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="2">
+        <v>100</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N23" s="2" t="s">
@@ -7568,39 +7575,39 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>50</v>
+    <row r="24" spans="1:32" s="1" customFormat="1" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>61</v>
+        <v>345</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>124</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="13">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="2">
+        <v>100</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>34</v>
@@ -7663,27 +7670,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:32" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" s="1" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>249</v>
+        <v>347</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>304</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>63</v>
@@ -7694,13 +7701,13 @@
       <c r="J25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="7" t="s">
-        <v>232</v>
+      <c r="K25" s="8" t="s">
+        <v>218</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="M25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N25" s="2" t="s">
@@ -7758,27 +7765,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" ht="395.25" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>83</v>
+        <v>349</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>304</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>63</v>
@@ -7789,8 +7796,8 @@
       <c r="J26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="7" t="s">
-        <v>139</v>
+      <c r="K26" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>34</v>
@@ -7854,27 +7861,27 @@
       </c>
       <c r="AF26"/>
     </row>
-    <row r="27" spans="1:32" s="43" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" s="43" customFormat="1" ht="279" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>250</v>
+        <v>350</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>304</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>63</v>
@@ -7885,13 +7892,13 @@
       <c r="J27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="7" t="s">
-        <v>232</v>
+      <c r="K27" s="8" t="s">
+        <v>217</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -7949,39 +7956,39 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>229</v>
+    <row r="28" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A28" s="33" t="s">
+        <v>268</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="D28" s="44" t="s">
         <v>304</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" s="2">
-        <v>100</v>
+        <v>272</v>
+      </c>
+      <c r="H28" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="36">
+        <v>1</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="7" t="s">
-        <v>139</v>
+      <c r="K28" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>34</v>
@@ -7999,13 +8006,13 @@
         <v>34</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="T28" s="2" t="s">
         <v>79</v>
@@ -8045,44 +8052,44 @@
       </c>
       <c r="AF28"/>
     </row>
-    <row r="29" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>133</v>
+        <v>38</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>126</v>
+        <v>308</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="13">
+        <v>1</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N29" s="2" t="s">
@@ -8141,39 +8148,39 @@
       </c>
       <c r="AF29"/>
     </row>
-    <row r="30" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
-        <v>57</v>
+    <row r="30" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>122</v>
+        <v>311</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="13">
+        <v>1</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>214</v>
+        <v>90</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>34</v>
@@ -8237,39 +8244,39 @@
       </c>
       <c r="AF30"/>
     </row>
-    <row r="31" spans="1:32" ht="186" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>120</v>
+        <v>312</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13">
+        <v>1</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>34</v>
@@ -8287,13 +8294,13 @@
         <v>34</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T31" s="2" t="s">
         <v>79</v>
@@ -8333,39 +8340,39 @@
       </c>
       <c r="AF31"/>
     </row>
-    <row r="32" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
-        <v>53</v>
+    <row r="32" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>130</v>
+        <v>313</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13">
+        <v>1</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>34</v>
@@ -8383,13 +8390,13 @@
         <v>34</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T32" s="2" t="s">
         <v>79</v>
@@ -8429,39 +8436,39 @@
       </c>
       <c r="AF32"/>
     </row>
-    <row r="33" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="22" t="s">
-        <v>55</v>
+    <row r="33" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>128</v>
+        <v>314</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I33" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13">
+        <v>1</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>212</v>
+        <v>90</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>34</v>
@@ -8479,13 +8486,13 @@
         <v>34</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T33" s="2" t="s">
         <v>79</v>
@@ -8525,39 +8532,39 @@
       </c>
       <c r="AF33"/>
     </row>
-    <row r="34" spans="1:32" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
-        <v>54</v>
+    <row r="34" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>129</v>
+        <v>315</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I34" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="13">
+        <v>1</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>211</v>
+        <v>90</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>34</v>
@@ -8575,13 +8582,13 @@
         <v>34</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T34" s="2" t="s">
         <v>79</v>
@@ -8621,39 +8628,39 @@
       </c>
       <c r="AF34"/>
     </row>
-    <row r="35" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
-      <c r="A35" s="22" t="s">
-        <v>56</v>
+    <row r="35" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>127</v>
+        <v>316</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I35" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13">
+        <v>1</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>213</v>
+        <v>90</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>34</v>
@@ -8671,13 +8678,13 @@
         <v>34</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T35" s="2" t="s">
         <v>79</v>
@@ -8717,39 +8724,39 @@
       </c>
       <c r="AF35"/>
     </row>
-    <row r="36" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A36" s="22" t="s">
-        <v>58</v>
+    <row r="36" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>123</v>
+        <v>317</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="13">
+        <v>1</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>34</v>
@@ -8813,39 +8820,39 @@
       </c>
       <c r="AF36"/>
     </row>
-    <row r="37" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="13">
+        <v>1</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>14</v>
+        <v>183</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>34</v>
@@ -8863,13 +8870,13 @@
         <v>34</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T37" s="2" t="s">
         <v>79</v>
@@ -8909,44 +8916,44 @@
       </c>
       <c r="AF37"/>
     </row>
-    <row r="38" spans="1:32" ht="348.75" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>135</v>
+        <v>318</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I38" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="13">
+        <v>1</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>219</v>
+        <v>90</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="M38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N38" s="2" t="s">
@@ -9007,36 +9014,36 @@
     </row>
     <row r="39" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>149</v>
+        <v>323</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>14</v>
+        <v>183</v>
       </c>
       <c r="I39" s="13">
         <v>1</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K39" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>90</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -9055,13 +9062,13 @@
         <v>34</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>79</v>
@@ -9101,39 +9108,39 @@
       </c>
       <c r="AF39"/>
     </row>
-    <row r="40" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="22" t="s">
-        <v>59</v>
+    <row r="40" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>124</v>
+        <v>319</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I40" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="13">
+        <v>1</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>216</v>
+        <v>90</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>34</v>
@@ -9197,39 +9204,39 @@
       </c>
       <c r="AF40"/>
     </row>
-    <row r="41" spans="1:32" ht="93" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I41" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="13">
+        <v>1</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>34</v>
@@ -9295,42 +9302,42 @@
     </row>
     <row r="42" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>132</v>
+        <v>321</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I42" s="2">
-        <v>100</v>
+        <v>184</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="13">
+        <v>1</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>218</v>
+        <v>16</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M42" s="3" t="s">
+      <c r="M42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N42" s="2" t="s">
@@ -9389,39 +9396,39 @@
       </c>
       <c r="AF42"/>
     </row>
-    <row r="43" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
-        <v>147</v>
+    <row r="43" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A43" s="33" t="s">
+        <v>259</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>306</v>
+        <v>359</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>299</v>
+        <v>301</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I43" s="13">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I43" s="36">
+        <v>1</v>
       </c>
       <c r="J43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="7" t="s">
-        <v>150</v>
+      <c r="K43" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>34</v>
@@ -9487,28 +9494,28 @@
     </row>
     <row r="44" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A44" s="33" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>270</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>304</v>
+        <v>362</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>290</v>
+        <v>301</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H44" s="36" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="I44" s="36">
         <v>1</v>
@@ -9517,7 +9524,7 @@
         <v>14</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>90</v>
+        <v>278</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>34</v>
@@ -9535,13 +9542,13 @@
         <v>34</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="T44" s="2" t="s">
         <v>79</v>
@@ -9581,39 +9588,39 @@
       </c>
       <c r="AF44"/>
     </row>
-    <row r="45" spans="1:32" ht="395.25" x14ac:dyDescent="0.35">
-      <c r="A45" s="12" t="s">
-        <v>8</v>
+    <row r="45" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A45" s="33" t="s">
+        <v>253</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>304</v>
+        <v>361</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="D45" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>290</v>
+        <v>301</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I45" s="2">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I45" s="36">
+        <v>1</v>
       </c>
       <c r="J45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K45" s="8" t="s">
-        <v>221</v>
+      <c r="K45" s="35" t="s">
+        <v>279</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>34</v>
@@ -9677,39 +9684,39 @@
       </c>
       <c r="AF45"/>
     </row>
-    <row r="46" spans="1:32" ht="93" x14ac:dyDescent="0.35">
-      <c r="A46" s="12" t="s">
-        <v>9</v>
+    <row r="46" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A46" s="33" t="s">
+        <v>254</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>304</v>
+        <v>360</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>289</v>
+        <v>301</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I46" s="2">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I46" s="36">
+        <v>1</v>
       </c>
       <c r="J46" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="7" t="s">
-        <v>137</v>
+      <c r="K46" s="35" t="s">
+        <v>280</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>34</v>
@@ -9773,44 +9780,44 @@
       </c>
       <c r="AF46"/>
     </row>
-    <row r="47" spans="1:32" ht="279" x14ac:dyDescent="0.35">
-      <c r="A47" s="12" t="s">
-        <v>9</v>
+    <row r="47" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A47" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>304</v>
+        <v>363</v>
+      </c>
+      <c r="C47" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>290</v>
+        <v>301</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I47" s="2">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H47" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I47" s="36">
+        <v>1</v>
       </c>
       <c r="J47" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K47" s="8" t="s">
-        <v>217</v>
+      <c r="K47" s="35" t="s">
+        <v>281</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M47" s="3" t="s">
+      <c r="M47" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N47" s="2" t="s">
@@ -9869,39 +9876,39 @@
       </c>
       <c r="AF47"/>
     </row>
-    <row r="48" spans="1:32" ht="209.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="12" t="s">
-        <v>28</v>
+    <row r="48" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A48" s="33" t="s">
+        <v>256</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>306</v>
+        <v>364</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>293</v>
+        <v>301</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I48" s="2">
+        <v>273</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I48" s="36">
         <v>1</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>161</v>
+      <c r="J48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K48" s="35" t="s">
+        <v>282</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>34</v>
@@ -9965,39 +9972,39 @@
       </c>
       <c r="AF48"/>
     </row>
-    <row r="49" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="12" t="s">
-        <v>29</v>
+    <row r="49" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A49" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>306</v>
+        <v>365</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>307</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>294</v>
+        <v>301</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I49" s="13">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H49" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I49" s="36">
+        <v>1</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K49" s="7" t="s">
-        <v>163</v>
+      <c r="K49" s="35" t="s">
+        <v>283</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>34</v>
@@ -10061,39 +10068,39 @@
       </c>
       <c r="AF49"/>
     </row>
-    <row r="50" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A50" s="12" t="s">
-        <v>30</v>
+    <row r="50" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A50" s="33" t="s">
+        <v>258</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>306</v>
+        <v>366</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>307</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>295</v>
+        <v>301</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I50" s="13">
-        <v>100</v>
+        <v>273</v>
+      </c>
+      <c r="H50" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I50" s="36">
+        <v>1</v>
       </c>
       <c r="J50" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K50" s="7" t="s">
-        <v>164</v>
+      <c r="K50" s="35" t="s">
+        <v>284</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>34</v>
@@ -10159,13 +10166,13 @@
     </row>
     <row r="51" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>306</v>
@@ -10174,10 +10181,10 @@
         <v>238</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>63</v>
@@ -10189,7 +10196,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>34</v>
@@ -10253,15 +10260,15 @@
       </c>
       <c r="AF51"/>
     </row>
-    <row r="52" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:32" ht="209.25" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D52" s="23" t="s">
         <v>306</v>
@@ -10270,22 +10277,22 @@
         <v>238</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I52" s="13">
-        <v>100</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>14</v>
+        <v>153</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>34</v>
@@ -10351,13 +10358,13 @@
     </row>
     <row r="53" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>306</v>
@@ -10366,7 +10373,7 @@
         <v>238</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>155</v>
@@ -10381,7 +10388,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>34</v>
@@ -10447,13 +10454,13 @@
     </row>
     <row r="54" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="D54" s="23" t="s">
         <v>306</v>
@@ -10462,22 +10469,22 @@
         <v>238</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H54" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="13">
         <v>100</v>
       </c>
       <c r="J54" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>34</v>
@@ -10541,39 +10548,39 @@
       </c>
       <c r="AF54"/>
     </row>
-    <row r="55" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A55" s="33" t="s">
-        <v>259</v>
+    <row r="55" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A55" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>359</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>267</v>
-      </c>
-      <c r="D55" s="44" t="s">
-        <v>307</v>
+        <v>354</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>306</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="F55" s="35" t="s">
-        <v>274</v>
+        <v>238</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H55" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I55" s="36">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I55" s="13">
+        <v>100</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K55" s="35" t="s">
-        <v>47</v>
+      <c r="K55" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>34</v>
@@ -10637,39 +10644,39 @@
       </c>
       <c r="AF55"/>
     </row>
-    <row r="56" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A56" s="33" t="s">
-        <v>252</v>
+    <row r="56" spans="1:32" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="A56" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="B56" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>260</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>307</v>
+        <v>357</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>306</v>
       </c>
       <c r="E56" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="F56" s="35" t="s">
-        <v>274</v>
+        <v>238</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>298</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H56" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I56" s="36">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="13">
+        <v>100</v>
       </c>
       <c r="J56" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K56" s="35" t="s">
-        <v>278</v>
+      <c r="K56" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>34</v>
@@ -10733,39 +10740,39 @@
       </c>
       <c r="AF56"/>
     </row>
-    <row r="57" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A57" s="33" t="s">
-        <v>253</v>
+    <row r="57" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A57" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>361</v>
-      </c>
-      <c r="C57" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="D57" s="44" t="s">
-        <v>307</v>
+        <v>353</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>306</v>
       </c>
       <c r="E57" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="F57" s="35" t="s">
-        <v>274</v>
+        <v>238</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H57" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I57" s="36">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" s="13">
+        <v>100</v>
       </c>
       <c r="J57" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K57" s="35" t="s">
-        <v>279</v>
+      <c r="K57" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>34</v>
@@ -10829,39 +10836,39 @@
       </c>
       <c r="AF57"/>
     </row>
-    <row r="58" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A58" s="33" t="s">
-        <v>254</v>
+    <row r="58" spans="1:32" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>360</v>
-      </c>
-      <c r="C58" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>307</v>
+        <v>358</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>306</v>
       </c>
       <c r="E58" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="F58" s="35" t="s">
-        <v>274</v>
+        <v>238</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>300</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I58" s="36">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="2">
+        <v>100</v>
       </c>
       <c r="J58" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K58" s="35" t="s">
-        <v>280</v>
+      <c r="K58" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>34</v>
@@ -10925,39 +10932,39 @@
       </c>
       <c r="AF58"/>
     </row>
-    <row r="59" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A59" s="33" t="s">
-        <v>255</v>
+    <row r="59" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>263</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>307</v>
+        <v>326</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F59" s="35" t="s">
-        <v>274</v>
+        <v>225</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H59" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I59" s="36">
+        <v>106</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I59" s="13">
         <v>1</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K59" s="35" t="s">
-        <v>281</v>
+        <v>107</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>34</v>
@@ -11021,39 +11028,39 @@
       </c>
       <c r="AF59"/>
     </row>
-    <row r="60" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A60" s="33" t="s">
-        <v>256</v>
+    <row r="60" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>264</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>307</v>
+        <v>327</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F60" s="35" t="s">
-        <v>274</v>
+        <v>225</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H60" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I60" s="36">
+        <v>106</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I60" s="13">
         <v>1</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K60" s="35" t="s">
-        <v>282</v>
+        <v>107</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>34</v>
@@ -11117,39 +11124,39 @@
       </c>
       <c r="AF60"/>
     </row>
-    <row r="61" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A61" s="33" t="s">
-        <v>257</v>
+    <row r="61" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>307</v>
+        <v>328</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F61" s="35" t="s">
-        <v>274</v>
+        <v>225</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H61" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I61" s="36">
+        <v>106</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I61" s="13">
         <v>1</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K61" s="35" t="s">
-        <v>283</v>
+        <v>107</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>34</v>
@@ -11213,39 +11220,39 @@
       </c>
       <c r="AF61"/>
     </row>
-    <row r="62" spans="1:32" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A62" s="33" t="s">
-        <v>258</v>
+    <row r="62" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="C62" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="D62" s="45" t="s">
-        <v>307</v>
+        <v>329</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F62" s="35" t="s">
-        <v>274</v>
+        <v>225</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="H62" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="I62" s="36">
+        <v>106</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I62" s="13">
         <v>1</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K62" s="35" t="s">
-        <v>284</v>
+        <v>107</v>
+      </c>
+      <c r="K62" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>34</v>
@@ -11311,43 +11318,43 @@
     </row>
     <row r="63" spans="1:32" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>95</v>
+        <v>330</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>290</v>
+        <v>47</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I63" s="2">
+        <v>106</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I63" s="13">
         <v>1</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>78</v>
+        <v>107</v>
+      </c>
+      <c r="K63" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>34</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>34</v>
@@ -11801,7 +11808,7 @@
       <c r="C6" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="45" t="s">
         <v>195</v>
       </c>
       <c r="E6" s="30" t="s">

</xml_diff>